<commit_message>
Modification BD + Realisation Manager + Fonctions + Page Accueil + Page Creer Annonce
</commit_message>
<xml_diff>
--- a/docs/Analysis/AG_PlanificationProjet.xlsx
+++ b/docs/Analysis/AG_PlanificationProjet.xlsx
@@ -610,7 +610,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="513">
+  <dxfs count="333">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -640,18 +640,46 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1332,34 +1360,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1407,6 +1407,27 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1447,6 +1468,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1480,6 +1508,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1612,27 +1647,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1668,6 +1682,60 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1791,1479 +1859,6 @@
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6384,690 +4979,690 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F43 H43:I43 I37 I40 G36:G37 H36 H38:H39 D9:D10 H51:I53 F51:F53 G40:G54 I42:I54 L36:L44 E36:E54 C36:C54 E3:E5 E7:E15 C3:C5 C7:C8 I3:I5 I7:I34 G3:G5 G7:G32 L3:L5 L7:L34 C11:C34 E18:E34 L48 L51:L54">
-    <cfRule type="cellIs" dxfId="512" priority="205" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="332" priority="205" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C54 E54:M54 C38:E38 C39:F39 H39 C40:M40 C37:M37 J36:M36 C43:M43 I33:M34 C33:F34 C36:H36 G38:H38 C41:G42 I42 F16:M17 D9:M10 E15:M15 C51:M51 C52:L53 C44:G50 I48:M48 C4:M5 C7:M8 C11:M13 E18:M18 C15:C18 C19:M32 K38:M39 L41:M42 I44:J44 L44 I45:K47 I49:K50">
-    <cfRule type="cellIs" dxfId="511" priority="204" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="331" priority="204" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:K54 F54 H54 M54">
-    <cfRule type="cellIs" dxfId="510" priority="201" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="330" priority="201" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43 G43 J43:K43 J51:K53 G51:G53 D51:D53">
-    <cfRule type="cellIs" dxfId="509" priority="200" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="329" priority="200" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54 E54:M54 C38:E38 C39:F39 H39 C40:M40 C37:M37 J36:M36 C43:M43 I33:M34 C33:F34 C36:H36 G38:H38 C41:G42 I42 F16:M17 C11:M13 D9:M10 C51:M51 C52:L53 C44:G50 I48:M48 C2:M5 C7:M8 E14:M15 E18:M18 C12:C18 C19:M32 K38:M39 L41:M42 I44:J44 L44 I45:K47 I49:K50">
-    <cfRule type="cellIs" dxfId="508" priority="197" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="507" priority="198" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="506" priority="199" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="328" priority="197" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="327" priority="198" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="326" priority="199" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N56">
-    <cfRule type="cellIs" dxfId="505" priority="190" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="325" priority="190" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="504" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="324" priority="196" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="503" priority="192" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="323" priority="192" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="502" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="322" priority="194" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:M57">
-    <cfRule type="cellIs" dxfId="501" priority="191" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="321" priority="191" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="500" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="193" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="499" priority="187" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="319" priority="187" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:J53">
-    <cfRule type="cellIs" dxfId="498" priority="186" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="318" priority="186" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:K53">
-    <cfRule type="cellIs" dxfId="497" priority="185" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="317" priority="185" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E56 C55:C56 G55:G56 I55:I56 L55">
-    <cfRule type="cellIs" dxfId="496" priority="179" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="316" priority="179" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:M55 C56:K56 M56">
-    <cfRule type="cellIs" dxfId="495" priority="178" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="315" priority="178" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:M55 C56:K56 M56">
-    <cfRule type="cellIs" dxfId="494" priority="175" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="493" priority="176" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="492" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="314" priority="175" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="313" priority="176" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="312" priority="177" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="491" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="311" priority="169" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55">
-    <cfRule type="cellIs" dxfId="490" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="310" priority="168" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55">
-    <cfRule type="cellIs" dxfId="489" priority="167" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="309" priority="167" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="488" priority="166" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="308" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="487" priority="163" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="486" priority="164" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="485" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="307" priority="163" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="306" priority="164" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="305" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55">
-    <cfRule type="cellIs" dxfId="484" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="304" priority="162" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="483" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="303" priority="161" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="482" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="302" priority="160" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="481" priority="157" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="480" priority="158" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="479" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="301" priority="157" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="300" priority="158" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="299" priority="159" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="478" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="298" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="477" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="297" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="476" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="296" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44:M45">
-    <cfRule type="cellIs" dxfId="475" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="295" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44:M45">
-    <cfRule type="cellIs" dxfId="474" priority="141" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="473" priority="142" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="472" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="294" priority="141" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="293" priority="142" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="292" priority="143" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46:M47">
-    <cfRule type="cellIs" dxfId="471" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="291" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46:M47">
-    <cfRule type="cellIs" dxfId="470" priority="137" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="469" priority="138" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="468" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="290" priority="137" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="289" priority="138" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="288" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M50">
-    <cfRule type="cellIs" dxfId="467" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="287" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M50">
-    <cfRule type="cellIs" dxfId="466" priority="129" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="465" priority="130" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="464" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="286" priority="129" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="285" priority="130" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="284" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M53">
-    <cfRule type="cellIs" dxfId="463" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="283" priority="128" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M53">
-    <cfRule type="cellIs" dxfId="462" priority="125" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="461" priority="126" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="460" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="282" priority="125" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="281" priority="126" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="280" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52">
-    <cfRule type="cellIs" dxfId="459" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="279" priority="124" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52">
-    <cfRule type="cellIs" dxfId="458" priority="121" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="457" priority="122" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="456" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="278" priority="121" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="277" priority="122" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="276" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35 I35 L35 E35 C35">
-    <cfRule type="cellIs" dxfId="455" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="275" priority="112" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:G35 I35:M35">
-    <cfRule type="cellIs" dxfId="454" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="274" priority="111" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:G35 I35:M35">
-    <cfRule type="cellIs" dxfId="453" priority="108" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="452" priority="109" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="451" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="273" priority="108" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="272" priority="109" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="271" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="450" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="270" priority="100" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="449" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="269" priority="99" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="448" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="268" priority="98" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="447" priority="95" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="446" priority="96" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="445" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="267" priority="95" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="266" priority="96" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="265" priority="97" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="444" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="264" priority="94" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="443" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="263" priority="93" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="442" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="262" priority="92" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="441" priority="91" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="261" priority="91" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="440" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="260" priority="90" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="439" priority="89" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="259" priority="89" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="438" priority="86" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="437" priority="87" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="436" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="258" priority="86" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="257" priority="87" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="256" priority="88" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="435" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="255" priority="85" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="434" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="254" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="433" priority="81" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="432" priority="82" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="431" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="253" priority="81" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="252" priority="82" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="251" priority="83" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="430" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="250" priority="80" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="429" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="249" priority="79" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="428" priority="76" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="427" priority="77" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="426" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="248" priority="76" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="247" priority="77" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="246" priority="78" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="425" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="245" priority="75" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="424" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="244" priority="74" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="423" priority="71" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="422" priority="72" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="421" priority="73" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="243" priority="71" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="242" priority="72" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="241" priority="73" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="420" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="240" priority="70" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="419" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="239" priority="69" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="418" priority="66" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="417" priority="67" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="416" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="238" priority="66" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="237" priority="67" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="236" priority="68" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="415" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="235" priority="65" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="414" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="234" priority="64" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="413" priority="61" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="412" priority="62" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="411" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="233" priority="61" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="232" priority="62" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="231" priority="63" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="410" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="230" priority="60" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="409" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="229" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="408" priority="56" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="407" priority="57" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="406" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="228" priority="56" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="227" priority="57" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="58" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="405" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="225" priority="55" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="404" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="224" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="403" priority="51" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="402" priority="52" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="401" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="223" priority="51" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="222" priority="52" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="221" priority="53" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="400" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="220" priority="50" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="399" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="219" priority="49" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="398" priority="46" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="397" priority="47" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="396" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="218" priority="46" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="47" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="216" priority="48" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="395" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="215" priority="45" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="394" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="214" priority="44" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="393" priority="41" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="392" priority="42" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="391" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="213" priority="41" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="212" priority="42" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="43" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="390" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="210" priority="40" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="389" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="209" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="388" priority="36" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="387" priority="37" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="386" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="208" priority="36" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="207" priority="37" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="206" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="385" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="205" priority="35" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="384" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="204" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="383" priority="31" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="382" priority="32" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="381" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="203" priority="31" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="202" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="201" priority="33" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="380" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="200" priority="30" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="379" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="199" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="378" priority="26" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="377" priority="27" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="376" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="198" priority="26" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="197" priority="27" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="375" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="195" priority="25" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="374" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="194" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="373" priority="21" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="372" priority="22" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="371" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="193" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="192" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="191" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="370" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="190" priority="20" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="369" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="189" priority="19" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="368" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="367" priority="17" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="366" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="188" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="187" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="186" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="365" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="185" priority="15" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="364" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="184" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="363" priority="11" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="362" priority="12" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="361" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="183" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="182" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="181" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="360" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="180" priority="10" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="359" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="179" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="358" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="357" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="356" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="178" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="177" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="355" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="175" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="354" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="174" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="353" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="352" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="351" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="173" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="172" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="171" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7081,7 +5676,7 @@
   <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7609,7 +6204,9 @@
       </c>
       <c r="C22" s="61"/>
       <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
+      <c r="E22" s="61">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F22" s="61"/>
       <c r="G22" s="61"/>
       <c r="H22" s="61"/>
@@ -7620,7 +6217,7 @@
       <c r="M22" s="61"/>
       <c r="N22" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -7632,7 +6229,9 @@
       </c>
       <c r="C23" s="61"/>
       <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
+      <c r="E23" s="61">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F23" s="61"/>
       <c r="G23" s="61"/>
       <c r="H23" s="61"/>
@@ -7643,7 +6242,7 @@
       <c r="M23" s="61"/>
       <c r="N23" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -7701,7 +6300,9 @@
       </c>
       <c r="C26" s="61"/>
       <c r="D26" s="53"/>
-      <c r="E26" s="61"/>
+      <c r="E26" s="61">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F26" s="53"/>
       <c r="G26" s="61"/>
       <c r="H26" s="53"/>
@@ -7712,7 +6313,7 @@
       <c r="M26" s="62"/>
       <c r="N26" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -7791,7 +6392,9 @@
       </c>
       <c r="C30" s="61"/>
       <c r="D30" s="53"/>
-      <c r="E30" s="61"/>
+      <c r="E30" s="61">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="F30" s="53"/>
       <c r="G30" s="53"/>
       <c r="H30" s="53"/>
@@ -7802,7 +6405,7 @@
       <c r="M30" s="62"/>
       <c r="N30" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -8099,7 +6702,9 @@
       </c>
       <c r="C44" s="61"/>
       <c r="D44" s="53"/>
-      <c r="E44" s="61"/>
+      <c r="E44" s="61">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F44" s="53"/>
       <c r="G44" s="61"/>
       <c r="I44" s="61"/>
@@ -8109,7 +6714,7 @@
       <c r="M44" s="62"/>
       <c r="N44" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -8121,7 +6726,9 @@
       </c>
       <c r="C45" s="61"/>
       <c r="D45" s="53"/>
-      <c r="E45" s="61"/>
+      <c r="E45" s="61">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F45" s="53"/>
       <c r="G45" s="61"/>
       <c r="I45" s="61"/>
@@ -8131,7 +6738,7 @@
       <c r="M45" s="62"/>
       <c r="N45" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -8418,7 +7025,7 @@
       </c>
       <c r="E57" s="77">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F57" s="77">
         <f t="shared" si="1"/>
@@ -8456,699 +7063,699 @@
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M58" s="3">
         <f>SUM(C57:M57)</f>
-        <v>1.75</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="N58" s="3">
         <f>SUM(N2:N56)</f>
-        <v>1.7499999999999998</v>
+        <v>1.9999999999999998</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F43 H43:I43 I37 I40 G36:G37 H36 H38:H39 D9:D10 H51:I53 F51:F53 G40:G54 I42 I44:I50 I54 L36:L44 E36:E54 C36:C54 E3:E5 E7:E11 C3:C5 C7:C8 I3:I5 I7:I11 G3:G5 G7:G11 L3:L5 L7:L11 E19:E34 L48 L51:L54 L19:L34 G19:G32 I19:I34 D12:M18 C11:C34 D21:M24">
-    <cfRule type="cellIs" dxfId="161" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="170" priority="162" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C54 E54:M54 C38:E38 C39:F39 H39 C40:M40 C37:M37 J36:M36 C43:M43 I33:M34 C33:F34 C36:H36 G38:H38 C41:G42 I42 D9:M10 C51:M51 C52:L53 C44:G50 I48:M48 C4:M5 C7:M8 K38:M39 L41:M42 I44:J44 L44 I45:K47 I49:K50 C11:M13 C15:M32">
-    <cfRule type="cellIs" dxfId="160" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="169" priority="161" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:K54 F54 H54 M54">
-    <cfRule type="cellIs" dxfId="159" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="168" priority="160" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43 G43 J43:K43 J51:K53 G51:G53 D51:D53">
-    <cfRule type="cellIs" dxfId="158" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="167" priority="159" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54 E54:M54 C38:E38 C39:F39 H39 C40:M40 C37:M37 J36:M36 C43:M43 I33:M34 C33:F34 C36:H36 G38:H38 C41:G42 I42 D9:M10 C51:M51 C52:L53 C44:G50 I48:M48 C2:M5 C7:M8 K38:M39 L41:M42 I44:J44 L44 I45:K47 I49:K50 C11:M32">
-    <cfRule type="cellIs" dxfId="157" priority="156" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="157" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="166" priority="156" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="165" priority="157" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="158" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N56">
-    <cfRule type="cellIs" dxfId="154" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="163" priority="150" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="155" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="152" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="161" priority="152" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="154" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:M57">
-    <cfRule type="cellIs" dxfId="150" priority="151" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="159" priority="151" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="153" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="148" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="157" priority="149" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:J53">
-    <cfRule type="cellIs" dxfId="147" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="156" priority="148" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:K53">
-    <cfRule type="cellIs" dxfId="146" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="155" priority="147" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E56 C55:C56 G55:G56 I55:I56 L55">
-    <cfRule type="cellIs" dxfId="145" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="154" priority="146" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:M55 C56:K56 M56">
-    <cfRule type="cellIs" dxfId="144" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="153" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:M55 C56:K56 M56">
-    <cfRule type="cellIs" dxfId="143" priority="142" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="143" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="152" priority="142" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="143" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="140" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="149" priority="141" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55">
-    <cfRule type="cellIs" dxfId="139" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="140" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55">
-    <cfRule type="cellIs" dxfId="138" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="139" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="137" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="146" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="136" priority="135" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="136" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="135" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="136" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="143" priority="137" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55">
-    <cfRule type="cellIs" dxfId="133" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="134" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="132" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="141" priority="133" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="131" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="130" priority="129" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="130" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="129" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="130" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="127" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="136" priority="128" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="126" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="125" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44:M45">
-    <cfRule type="cellIs" dxfId="124" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44:M45">
-    <cfRule type="cellIs" dxfId="123" priority="122" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="123" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="122" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="123" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="124" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46:M47">
-    <cfRule type="cellIs" dxfId="120" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46:M47">
-    <cfRule type="cellIs" dxfId="119" priority="118" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="119" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="118" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="119" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M50">
-    <cfRule type="cellIs" dxfId="116" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="117" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M50">
-    <cfRule type="cellIs" dxfId="115" priority="114" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="115" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="114" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="115" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M53">
-    <cfRule type="cellIs" dxfId="112" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M53">
-    <cfRule type="cellIs" dxfId="111" priority="110" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="111" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="120" priority="110" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="111" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52">
-    <cfRule type="cellIs" dxfId="108" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="117" priority="109" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52">
-    <cfRule type="cellIs" dxfId="107" priority="106" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="107" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="106" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="107" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="108" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35 I35 L35 E35 C35">
-    <cfRule type="cellIs" dxfId="104" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="105" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:G35 I35:M35">
-    <cfRule type="cellIs" dxfId="103" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="104" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:G35 I35:M35">
-    <cfRule type="cellIs" dxfId="102" priority="101" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="102" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="101" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="102" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="109" priority="103" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="99" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="100" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="98" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="99" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="97" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="98" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="96" priority="95" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="96" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="95" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="96" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="103" priority="97" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="93" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="94" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="92" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="93" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="91" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="92" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="90" priority="91" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="91" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="89" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="90" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="88" priority="89" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="89" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="87" priority="86" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="87" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="86" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="87" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="88" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="84" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="85" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="83" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="82" priority="81" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="82" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="81" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="82" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="83" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="79" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="80" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="78" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="79" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="77" priority="76" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="77" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="76" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="77" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="78" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="74" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="75" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="73" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="74" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="72" priority="71" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="72" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="73" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="71" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="72" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="73" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="69" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="70" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="68" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="69" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="67" priority="66" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="67" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="66" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="67" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="68" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="64" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="65" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="64" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="62" priority="61" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="62" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="61" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="62" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="63" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="59" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="60" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="58" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="57" priority="56" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="57" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="56" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="57" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="58" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="55" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="53" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="52" priority="51" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="52" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="51" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="52" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="53" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="50" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="49" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="47" priority="46" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="46" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="47" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="48" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="44" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="45" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="43" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="44" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="42" priority="41" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="42" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="41" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="42" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="43" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="40" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="37" priority="36" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="36" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="37" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="35" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="33" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="31" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="33" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="30" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="26" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="27" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="25" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="19" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="15" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9886,43 +8493,43 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:L2 F24 H24:I24 C3:C20 E3:E20 G3:G20 I3:I20 K3:K20 C22:C26 G22:G26 I22:I23 I25:I26 E22:E26 K22:K26">
-    <cfRule type="cellIs" dxfId="170" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L2 C4:L11 C13:L20 C22:L26">
-    <cfRule type="cellIs" dxfId="169" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="168" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:L21">
-    <cfRule type="cellIs" dxfId="167" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25 F25 H25 J25 L25">
-    <cfRule type="cellIs" dxfId="166" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24 G24 J24">
-    <cfRule type="cellIs" dxfId="165" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L26">
-    <cfRule type="cellIs" dxfId="164" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Creation d'annonces + realisation doc + creation page details annonce + creation page mes annonces + creation page modification d'annnonces
</commit_message>
<xml_diff>
--- a/docs/Analysis/AG_PlanificationProjet.xlsx
+++ b/docs/Analysis/AG_PlanificationProjet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="82">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -258,6 +258,15 @@
   </si>
   <si>
     <t>Implémentation du MCD + Création des classes associées</t>
+  </si>
+  <si>
+    <t>Page de détails d'une annonce</t>
+  </si>
+  <si>
+    <t>Affichage détails d'une annonce</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -3540,7 +3549,7 @@
   <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A60" sqref="A1:XFD1048576"/>
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5673,10 +5682,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5772,7 +5781,7 @@
       <c r="L3" s="58"/>
       <c r="M3" s="60"/>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N56" si="0">SUM(C3:M3)</f>
+        <f t="shared" ref="N3:N58" si="0">SUM(C3:M3)</f>
         <v>0</v>
       </c>
     </row>
@@ -6303,7 +6312,9 @@
       <c r="E26" s="61">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F26" s="53"/>
+      <c r="F26" s="53">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G26" s="61"/>
       <c r="H26" s="53"/>
       <c r="I26" s="61"/>
@@ -6313,7 +6324,7 @@
       <c r="M26" s="62"/>
       <c r="N26" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -6395,7 +6406,9 @@
       <c r="E30" s="61">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F30" s="53"/>
+      <c r="F30" s="53">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G30" s="53"/>
       <c r="H30" s="53"/>
       <c r="I30" s="61"/>
@@ -6405,7 +6418,7 @@
       <c r="M30" s="62"/>
       <c r="N30" s="3">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -6454,39 +6467,42 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="45" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B33" s="34">
-        <v>0.16666666666666666</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C33" s="61"/>
       <c r="D33" s="53"/>
       <c r="E33" s="61"/>
-      <c r="F33" s="53"/>
+      <c r="F33" s="53">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
+      <c r="H33" s="53"/>
       <c r="I33" s="61"/>
       <c r="J33" s="53"/>
       <c r="K33" s="53"/>
       <c r="L33" s="61"/>
       <c r="M33" s="62"/>
-      <c r="N33" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="45" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B34" s="34">
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C34" s="61"/>
       <c r="D34" s="53"/>
       <c r="E34" s="61"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="61"/>
+      <c r="F34" s="53">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G34" s="61" t="s">
+        <v>81</v>
+      </c>
       <c r="H34" s="61"/>
       <c r="I34" s="61"/>
       <c r="J34" s="53"/>
@@ -6495,22 +6511,22 @@
       <c r="M34" s="62"/>
       <c r="N34" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
-        <v>63</v>
+      <c r="A35" s="45" t="s">
+        <v>72</v>
       </c>
       <c r="B35" s="34">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C35" s="61"/>
       <c r="D35" s="53"/>
       <c r="E35" s="61"/>
       <c r="F35" s="53"/>
       <c r="G35" s="61"/>
-      <c r="H35" s="53"/>
+      <c r="H35" s="61"/>
       <c r="I35" s="61"/>
       <c r="J35" s="53"/>
       <c r="K35" s="53"/>
@@ -6522,18 +6538,20 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>57</v>
+      <c r="A36" s="46" t="s">
+        <v>63</v>
       </c>
       <c r="B36" s="34">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C36" s="61"/>
       <c r="D36" s="53"/>
       <c r="E36" s="61"/>
-      <c r="F36" s="53"/>
+      <c r="F36" s="53">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
+      <c r="H36" s="53"/>
       <c r="I36" s="61"/>
       <c r="J36" s="53"/>
       <c r="K36" s="53"/>
@@ -6541,46 +6559,48 @@
       <c r="M36" s="62"/>
       <c r="N36" s="3">
         <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="34">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C37" s="61"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="61"/>
+      <c r="M37" s="62"/>
+      <c r="N37" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="50" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="49"/>
-      <c r="C37" s="66"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="67"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="67"/>
-      <c r="K37" s="67"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="68"/>
-      <c r="N37" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="43">
-        <v>0.125</v>
-      </c>
-      <c r="C38" s="61"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="61"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="61"/>
-      <c r="I38" s="61"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="62"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="66"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="67"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="68"/>
       <c r="N38" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6588,7 +6608,7 @@
     </row>
     <row r="39" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B39" s="43">
         <v>0.125</v>
@@ -6596,11 +6616,9 @@
       <c r="C39" s="61"/>
       <c r="D39" s="53"/>
       <c r="E39" s="61"/>
-      <c r="F39" s="53"/>
       <c r="G39" s="53"/>
       <c r="H39" s="61"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="61"/>
+      <c r="I39" s="61"/>
       <c r="K39" s="53"/>
       <c r="L39" s="61"/>
       <c r="M39" s="62"/>
@@ -6609,42 +6627,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="48" t="s">
+    <row r="40" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="43">
+        <v>0.125</v>
+      </c>
+      <c r="C40" s="61"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="61"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="61"/>
+      <c r="M40" s="62"/>
+      <c r="N40" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="49"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="66"/>
-      <c r="J40" s="67"/>
-      <c r="K40" s="67"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="68"/>
-      <c r="N40" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="34">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="61"/>
-      <c r="J41" s="61"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="62"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="66"/>
+      <c r="J41" s="67"/>
+      <c r="K41" s="67"/>
+      <c r="L41" s="66"/>
+      <c r="M41" s="68"/>
       <c r="N41" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6652,19 +6673,17 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="34">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C42" s="61"/>
       <c r="D42" s="53"/>
       <c r="E42" s="61"/>
       <c r="F42" s="53"/>
       <c r="G42" s="61"/>
-      <c r="I42" s="61"/>
       <c r="J42" s="61"/>
-      <c r="K42" s="53"/>
       <c r="L42" s="61"/>
       <c r="M42" s="62"/>
       <c r="N42" s="3">
@@ -6673,56 +6692,54 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="52" t="s">
+      <c r="A43" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="34">
+        <v>0.125</v>
+      </c>
+      <c r="C43" s="61"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="53"/>
+      <c r="L43" s="61"/>
+      <c r="M43" s="62"/>
+      <c r="N43" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="47"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="60"/>
-      <c r="N43" s="3">
+      <c r="B44" s="47"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="58"/>
+      <c r="L44" s="58"/>
+      <c r="M44" s="60"/>
+      <c r="N44" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="34">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C44" s="61"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="61">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F44" s="53"/>
-      <c r="G44" s="61"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="53"/>
-      <c r="L44" s="61"/>
-      <c r="M44" s="62"/>
-      <c r="N44" s="3">
-        <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45" s="34">
-        <v>4.1666666666666664E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C45" s="61"/>
       <c r="D45" s="53"/>
@@ -6734,7 +6751,7 @@
       <c r="I45" s="61"/>
       <c r="J45" s="53"/>
       <c r="K45" s="53"/>
-      <c r="L45" s="53"/>
+      <c r="L45" s="61"/>
       <c r="M45" s="62"/>
       <c r="N45" s="3">
         <f t="shared" si="0"/>
@@ -6742,15 +6759,17 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="41" t="s">
-        <v>46</v>
+      <c r="A46" s="38" t="s">
+        <v>49</v>
       </c>
       <c r="B46" s="34">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C46" s="61"/>
       <c r="D46" s="53"/>
-      <c r="E46" s="61"/>
+      <c r="E46" s="61">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F46" s="53"/>
       <c r="G46" s="61"/>
       <c r="I46" s="61"/>
@@ -6760,20 +6779,22 @@
       <c r="M46" s="62"/>
       <c r="N46" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="40" t="s">
-        <v>47</v>
+      <c r="A47" s="38" t="s">
+        <v>79</v>
       </c>
       <c r="B47" s="34">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C47" s="61"/>
       <c r="D47" s="53"/>
       <c r="E47" s="61"/>
-      <c r="F47" s="53"/>
+      <c r="F47" s="53">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G47" s="61"/>
       <c r="I47" s="61"/>
       <c r="J47" s="53"/>
@@ -6782,15 +6803,15 @@
       <c r="M47" s="62"/>
       <c r="N47" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
-        <v>69</v>
+      <c r="A48" s="41" t="s">
+        <v>46</v>
       </c>
       <c r="B48" s="34">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C48" s="61"/>
       <c r="D48" s="53"/>
@@ -6800,7 +6821,7 @@
       <c r="I48" s="61"/>
       <c r="J48" s="53"/>
       <c r="K48" s="53"/>
-      <c r="L48" s="61"/>
+      <c r="L48" s="53"/>
       <c r="M48" s="62"/>
       <c r="N48" s="3">
         <f t="shared" si="0"/>
@@ -6808,8 +6829,8 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="39" t="s">
-        <v>70</v>
+      <c r="A49" s="40" t="s">
+        <v>47</v>
       </c>
       <c r="B49" s="34">
         <v>4.1666666666666664E-2</v>
@@ -6831,10 +6852,10 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="39" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B50" s="34">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C50" s="61"/>
       <c r="D50" s="53"/>
@@ -6844,7 +6865,7 @@
       <c r="I50" s="61"/>
       <c r="J50" s="53"/>
       <c r="K50" s="53"/>
-      <c r="L50" s="53"/>
+      <c r="L50" s="61"/>
       <c r="M50" s="62"/>
       <c r="N50" s="3">
         <f t="shared" si="0"/>
@@ -6852,21 +6873,22 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" s="47"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-      <c r="J51" s="58"/>
-      <c r="K51" s="58"/>
-      <c r="L51" s="58"/>
-      <c r="M51" s="60"/>
+      <c r="A51" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C51" s="61"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="61"/>
+      <c r="I51" s="61"/>
+      <c r="J51" s="53"/>
+      <c r="K51" s="53"/>
+      <c r="L51" s="53"/>
+      <c r="M51" s="62"/>
       <c r="N51" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6874,224 +6896,267 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C52" s="61"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="61"/>
+      <c r="I52" s="61"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="53"/>
+      <c r="L52" s="53"/>
+      <c r="M52" s="62"/>
+      <c r="N52" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="47"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="58"/>
+      <c r="J53" s="58"/>
+      <c r="K53" s="58"/>
+      <c r="L53" s="58"/>
+      <c r="M53" s="60"/>
+      <c r="N53" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="34">
+      <c r="B54" s="34">
         <v>0.5</v>
       </c>
-      <c r="C52" s="61"/>
-      <c r="D52" s="61"/>
-      <c r="E52" s="61"/>
-      <c r="F52" s="61">
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="61">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="G54" s="61"/>
+      <c r="H54" s="61">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G52" s="61"/>
-      <c r="H52" s="61">
+      <c r="I54" s="61">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="I52" s="61">
+      <c r="J54" s="61"/>
+      <c r="K54" s="61">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="J52" s="61"/>
-      <c r="K52" s="61">
+      <c r="L54" s="61">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="L52" s="61">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M52" s="62">
+      <c r="M54" s="62">
         <v>0.29166666666666669</v>
       </c>
-      <c r="N52" s="3">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="39" t="s">
+      <c r="N54" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="43">
+      <c r="B55" s="43">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C53" s="61"/>
-      <c r="D53" s="61">
+      <c r="C55" s="61"/>
+      <c r="D55" s="61">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E53" s="61"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
-      <c r="H53" s="61"/>
-      <c r="I53" s="61"/>
-      <c r="J53" s="61"/>
-      <c r="K53" s="61"/>
-      <c r="L53" s="61"/>
-      <c r="M53" s="62"/>
-      <c r="N53" s="3">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" s="47"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="69"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="58"/>
-      <c r="K54" s="58"/>
-      <c r="L54" s="58"/>
-      <c r="M54" s="70"/>
-      <c r="N54" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="B55" s="34">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="C55" s="61"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="53">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="F55" s="53">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G55" s="53">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H55" s="53">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="I55" s="53">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J55" s="53">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="K55" s="53">
-        <v>0.125</v>
-      </c>
-      <c r="L55" s="53"/>
+      <c r="E55" s="61"/>
+      <c r="F55" s="61"/>
+      <c r="G55" s="61"/>
+      <c r="H55" s="61"/>
+      <c r="I55" s="61"/>
+      <c r="J55" s="61"/>
+      <c r="K55" s="61"/>
+      <c r="L55" s="61"/>
       <c r="M55" s="62"/>
       <c r="N55" s="3">
         <f t="shared" si="0"/>
-        <v>0.58333333333333326</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="41"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="61"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="61"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="61"/>
-      <c r="H56" s="53"/>
-      <c r="I56" s="61"/>
-      <c r="J56" s="53"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="61"/>
-      <c r="M56" s="62"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="47"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="58"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
+      <c r="I56" s="58"/>
+      <c r="J56" s="58"/>
+      <c r="K56" s="58"/>
+      <c r="L56" s="58"/>
+      <c r="M56" s="70"/>
       <c r="N56" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="76"/>
-      <c r="B57" s="77">
-        <f>SUM(B2:B56)</f>
-        <v>3.6666666666666661</v>
-      </c>
-      <c r="C57" s="77">
-        <f t="shared" ref="C57:M57" si="1">SUM(C2:C56)</f>
+      <c r="A57" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="34">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C57" s="61"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="53">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F57" s="53">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G57" s="53">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H57" s="53">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I57" s="53">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="J57" s="53">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K57" s="53">
+        <v>0.125</v>
+      </c>
+      <c r="L57" s="53"/>
+      <c r="M57" s="62"/>
+      <c r="N57" s="3">
+        <f t="shared" si="0"/>
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="41"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="61"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="61"/>
+      <c r="J58" s="53"/>
+      <c r="K58" s="53"/>
+      <c r="L58" s="61"/>
+      <c r="M58" s="62"/>
+      <c r="N58" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="76"/>
+      <c r="B59" s="77">
+        <f>SUM(B2:B58)</f>
+        <v>3.7291666666666665</v>
+      </c>
+      <c r="C59" s="77">
+        <f t="shared" ref="C59:M59" si="1">SUM(C2:C58)</f>
         <v>0.33333333333333326</v>
       </c>
-      <c r="D57" s="77">
+      <c r="D59" s="77">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E57" s="77">
+      <c r="E59" s="77">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F57" s="77">
+      <c r="F59" s="77">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="G59" s="77">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H59" s="77">
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="G57" s="77">
+      <c r="I59" s="77">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H57" s="77">
-        <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-      <c r="I57" s="77">
+      <c r="J59" s="77">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="J57" s="77">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="K57" s="77">
+      <c r="K59" s="77">
         <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="L57" s="77">
+      <c r="L59" s="77">
         <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="M57" s="77">
+      <c r="M59" s="77">
         <f t="shared" si="1"/>
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M58" s="3">
-        <f>SUM(C57:M57)</f>
-        <v>1.9999999999999998</v>
-      </c>
-      <c r="N58" s="3">
-        <f>SUM(N2:N56)</f>
-        <v>1.9999999999999998</v>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M60" s="3">
+        <f>SUM(C59:M59)</f>
+        <v>2.208333333333333</v>
+      </c>
+      <c r="N60" s="3">
+        <f>SUM(N2:N58)</f>
+        <v>2.1666666666666665</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:M2 F43 H43:I43 I37 I40 G36:G37 H36 H38:H39 D9:D10 H51:I53 F51:F53 G40:G54 I42 I44:I50 I54 L36:L44 E36:E54 C36:C54 E3:E5 E7:E11 C3:C5 C7:C8 I3:I5 I7:I11 G3:G5 G7:G11 L3:L5 L7:L11 E19:E34 L48 L51:L54 L19:L34 G19:G32 I19:I34 D12:M18 C11:C34 D21:M24">
+  <conditionalFormatting sqref="C2:M2 F44 H44:I44 I38 I41 G37:G38 H37 H39:H40 D9:D10 H53:I55 F53:F55 G41:G56 I43 I45:I52 I56 L37:L45 E37:E56 C37:C56 E3:E5 E7:E11 C3:C5 C7:C8 I3:I5 I7:I11 G3:G5 G7:G11 L3:L5 L7:L11 E19:E35 L50 L53:L56 L19:L35 G19:G33 I19:I35 D12:M18 C11:C35 D21:M24">
     <cfRule type="cellIs" dxfId="170" priority="162" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M2 C54 E54:M54 C38:E38 C39:F39 H39 C40:M40 C37:M37 J36:M36 C43:M43 I33:M34 C33:F34 C36:H36 G38:H38 C41:G42 I42 D9:M10 C51:M51 C52:L53 C44:G50 I48:M48 C4:M5 C7:M8 K38:M39 L41:M42 I44:J44 L44 I45:K47 I49:K50 C11:M13 C15:M32">
+  <conditionalFormatting sqref="C2:M2 C56 E56:M56 C39:E39 C40:F40 H40 C41:M41 C38:M38 J37:M37 C44:M44 I34:M35 C34:F35 C37:H37 G39:H39 C42:G43 I43 D9:M10 C53:M53 C54:L55 C45:G52 I50:M50 C4:M5 C7:M8 K39:M40 L42:M43 I45:J45 L45 I46:K49 I51:K52 C11:M13 C15:M33">
     <cfRule type="cellIs" dxfId="169" priority="161" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J54:K54 F54 H54 M54">
+  <conditionalFormatting sqref="J56:K56 F56 H56 M56">
     <cfRule type="cellIs" dxfId="168" priority="160" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43 G43 J43:K43 J51:K53 G51:G53 D51:D53">
+  <conditionalFormatting sqref="D44 G44 J44:K44 J53:K55 G53:G55 D53:D55">
     <cfRule type="cellIs" dxfId="167" priority="159" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54 E54:M54 C38:E38 C39:F39 H39 C40:M40 C37:M37 J36:M36 C43:M43 I33:M34 C33:F34 C36:H36 G38:H38 C41:G42 I42 D9:M10 C51:M51 C52:L53 C44:G50 I48:M48 C2:M5 C7:M8 K38:M39 L41:M42 I44:J44 L44 I45:K47 I49:K50 C11:M32">
+  <conditionalFormatting sqref="C56 E56:M56 C39:E39 C40:F40 H40 C41:M41 C38:M38 J37:M37 C44:M44 I34:M35 C34:F35 C37:H37 G39:H39 C42:G43 I43 D9:M10 C53:M53 C54:L55 C45:G52 I50:M50 C2:M5 C7:M8 K39:M40 L42:M43 I45:J45 L45 I46:K49 I51:K52 C11:M33">
     <cfRule type="cellIs" dxfId="166" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7102,7 +7167,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N56">
+  <conditionalFormatting sqref="N2:N58">
     <cfRule type="cellIs" dxfId="163" priority="150" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
@@ -7110,7 +7175,7 @@
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57">
+  <conditionalFormatting sqref="B59">
     <cfRule type="cellIs" dxfId="161" priority="152" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
@@ -7118,7 +7183,7 @@
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:M57">
+  <conditionalFormatting sqref="C59:M59">
     <cfRule type="cellIs" dxfId="159" priority="151" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
@@ -7131,27 +7196,27 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J52:J53">
+  <conditionalFormatting sqref="J54:J55">
     <cfRule type="cellIs" dxfId="156" priority="148" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K52:K53">
+  <conditionalFormatting sqref="K54:K55">
     <cfRule type="cellIs" dxfId="155" priority="147" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E55:E56 C55:C56 G55:G56 I55:I56 L55">
+  <conditionalFormatting sqref="E57:E58 C57:C58 G57:G58 I57:I58 L57">
     <cfRule type="cellIs" dxfId="154" priority="146" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55:M55 C56:K56 M56">
+  <conditionalFormatting sqref="C57:M57 C58:K58 M58">
     <cfRule type="cellIs" dxfId="153" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55:M55 C56:K56 M56">
+  <conditionalFormatting sqref="C57:M57 C58:K58 M58">
     <cfRule type="cellIs" dxfId="152" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7162,27 +7227,27 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55">
+  <conditionalFormatting sqref="H57">
     <cfRule type="cellIs" dxfId="149" priority="141" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J55">
+  <conditionalFormatting sqref="J57">
     <cfRule type="cellIs" dxfId="148" priority="140" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K55">
+  <conditionalFormatting sqref="K57">
     <cfRule type="cellIs" dxfId="147" priority="139" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G39">
+  <conditionalFormatting sqref="G40">
     <cfRule type="cellIs" dxfId="146" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G39">
+  <conditionalFormatting sqref="G40">
     <cfRule type="cellIs" dxfId="145" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7193,22 +7258,22 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F55">
+  <conditionalFormatting sqref="F57">
     <cfRule type="cellIs" dxfId="142" priority="134" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
+  <conditionalFormatting sqref="G35">
     <cfRule type="cellIs" dxfId="141" priority="133" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
+  <conditionalFormatting sqref="G35">
     <cfRule type="cellIs" dxfId="140" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
+  <conditionalFormatting sqref="G35">
     <cfRule type="cellIs" dxfId="139" priority="129" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7234,12 +7299,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M44:M45">
+  <conditionalFormatting sqref="M45:M47">
     <cfRule type="cellIs" dxfId="133" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M44:M45">
+  <conditionalFormatting sqref="M45:M47">
     <cfRule type="cellIs" dxfId="132" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7250,12 +7315,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M46:M47">
+  <conditionalFormatting sqref="M48:M49">
     <cfRule type="cellIs" dxfId="129" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M46:M47">
+  <conditionalFormatting sqref="M48:M49">
     <cfRule type="cellIs" dxfId="128" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7266,12 +7331,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M49:M50">
+  <conditionalFormatting sqref="M51:M52">
     <cfRule type="cellIs" dxfId="125" priority="117" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M49:M50">
+  <conditionalFormatting sqref="M51:M52">
     <cfRule type="cellIs" dxfId="124" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7282,12 +7347,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53">
+  <conditionalFormatting sqref="M55">
     <cfRule type="cellIs" dxfId="121" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53">
+  <conditionalFormatting sqref="M55">
     <cfRule type="cellIs" dxfId="120" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7298,12 +7363,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M52">
+  <conditionalFormatting sqref="M54">
     <cfRule type="cellIs" dxfId="117" priority="109" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M52">
+  <conditionalFormatting sqref="M54">
     <cfRule type="cellIs" dxfId="116" priority="106" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7314,17 +7379,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35 I35 L35 E35 C35">
+  <conditionalFormatting sqref="G36 I36 L36 E36 C36">
     <cfRule type="cellIs" dxfId="113" priority="105" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35:G35 I35:M35">
+  <conditionalFormatting sqref="C36:G36 I36:M36">
     <cfRule type="cellIs" dxfId="112" priority="104" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35:G35 I35:M35">
+  <conditionalFormatting sqref="C36:G36 I36:M36">
     <cfRule type="cellIs" dxfId="111" priority="101" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7381,17 +7446,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
+  <conditionalFormatting sqref="G34">
     <cfRule type="cellIs" dxfId="98" priority="90" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
+  <conditionalFormatting sqref="G34">
     <cfRule type="cellIs" dxfId="97" priority="89" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
+  <conditionalFormatting sqref="G34">
     <cfRule type="cellIs" dxfId="96" priority="86" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7402,17 +7467,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
+  <conditionalFormatting sqref="H34">
     <cfRule type="cellIs" dxfId="93" priority="85" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
+  <conditionalFormatting sqref="H34">
     <cfRule type="cellIs" dxfId="92" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
+  <conditionalFormatting sqref="H34">
     <cfRule type="cellIs" dxfId="91" priority="81" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7423,17 +7488,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
+  <conditionalFormatting sqref="H35">
     <cfRule type="cellIs" dxfId="88" priority="80" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
+  <conditionalFormatting sqref="H35">
     <cfRule type="cellIs" dxfId="87" priority="79" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
+  <conditionalFormatting sqref="H35">
     <cfRule type="cellIs" dxfId="86" priority="76" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7444,17 +7509,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+  <conditionalFormatting sqref="H36">
     <cfRule type="cellIs" dxfId="83" priority="75" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+  <conditionalFormatting sqref="H36">
     <cfRule type="cellIs" dxfId="82" priority="74" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+  <conditionalFormatting sqref="H36">
     <cfRule type="cellIs" dxfId="81" priority="71" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7465,17 +7530,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
+  <conditionalFormatting sqref="I37">
     <cfRule type="cellIs" dxfId="78" priority="70" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
+  <conditionalFormatting sqref="I37">
     <cfRule type="cellIs" dxfId="77" priority="69" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
+  <conditionalFormatting sqref="I37">
     <cfRule type="cellIs" dxfId="76" priority="66" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7486,17 +7551,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
+  <conditionalFormatting sqref="I39">
     <cfRule type="cellIs" dxfId="73" priority="65" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
+  <conditionalFormatting sqref="I39">
     <cfRule type="cellIs" dxfId="72" priority="64" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
+  <conditionalFormatting sqref="I39">
     <cfRule type="cellIs" dxfId="71" priority="61" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7507,17 +7572,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I40">
     <cfRule type="cellIs" dxfId="68" priority="60" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I40">
     <cfRule type="cellIs" dxfId="67" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I40">
     <cfRule type="cellIs" dxfId="66" priority="56" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7528,17 +7593,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J39">
+  <conditionalFormatting sqref="J40">
     <cfRule type="cellIs" dxfId="63" priority="55" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J39">
+  <conditionalFormatting sqref="J40">
     <cfRule type="cellIs" dxfId="62" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J39">
+  <conditionalFormatting sqref="J40">
     <cfRule type="cellIs" dxfId="61" priority="51" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7549,17 +7614,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J41">
+  <conditionalFormatting sqref="J42">
     <cfRule type="cellIs" dxfId="58" priority="50" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J41">
+  <conditionalFormatting sqref="J42">
     <cfRule type="cellIs" dxfId="57" priority="49" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J41">
+  <conditionalFormatting sqref="J42">
     <cfRule type="cellIs" dxfId="56" priority="46" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7570,17 +7635,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K42">
+  <conditionalFormatting sqref="K43">
     <cfRule type="cellIs" dxfId="53" priority="45" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K42">
+  <conditionalFormatting sqref="K43">
     <cfRule type="cellIs" dxfId="52" priority="44" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K42">
+  <conditionalFormatting sqref="K43">
     <cfRule type="cellIs" dxfId="51" priority="41" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7591,17 +7656,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
+  <conditionalFormatting sqref="J43">
     <cfRule type="cellIs" dxfId="48" priority="40" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
+  <conditionalFormatting sqref="J43">
     <cfRule type="cellIs" dxfId="47" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
+  <conditionalFormatting sqref="J43">
     <cfRule type="cellIs" dxfId="46" priority="36" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7612,17 +7677,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K44">
+  <conditionalFormatting sqref="K45">
     <cfRule type="cellIs" dxfId="43" priority="35" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K44">
+  <conditionalFormatting sqref="K45">
     <cfRule type="cellIs" dxfId="42" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K44">
+  <conditionalFormatting sqref="K45">
     <cfRule type="cellIs" dxfId="41" priority="31" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7633,17 +7698,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L45">
+  <conditionalFormatting sqref="L46:L47">
     <cfRule type="cellIs" dxfId="38" priority="30" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L45">
+  <conditionalFormatting sqref="L46:L47">
     <cfRule type="cellIs" dxfId="37" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L45">
+  <conditionalFormatting sqref="L46:L47">
     <cfRule type="cellIs" dxfId="36" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7654,17 +7719,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L46">
+  <conditionalFormatting sqref="L48">
     <cfRule type="cellIs" dxfId="33" priority="25" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L46">
+  <conditionalFormatting sqref="L48">
     <cfRule type="cellIs" dxfId="32" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L46">
+  <conditionalFormatting sqref="L48">
     <cfRule type="cellIs" dxfId="31" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7675,17 +7740,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L47">
+  <conditionalFormatting sqref="L49">
     <cfRule type="cellIs" dxfId="28" priority="20" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L47">
+  <conditionalFormatting sqref="L49">
     <cfRule type="cellIs" dxfId="27" priority="19" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L47">
+  <conditionalFormatting sqref="L49">
     <cfRule type="cellIs" dxfId="26" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7696,17 +7761,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L49">
+  <conditionalFormatting sqref="L51">
     <cfRule type="cellIs" dxfId="23" priority="15" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L49">
+  <conditionalFormatting sqref="L51">
     <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L49">
+  <conditionalFormatting sqref="L51">
     <cfRule type="cellIs" dxfId="21" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7717,17 +7782,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L50">
+  <conditionalFormatting sqref="L52">
     <cfRule type="cellIs" dxfId="18" priority="10" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L50">
+  <conditionalFormatting sqref="L52">
     <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L50">
+  <conditionalFormatting sqref="L52">
     <cfRule type="cellIs" dxfId="16" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7738,17 +7803,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L56">
+  <conditionalFormatting sqref="L58">
     <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L56">
+  <conditionalFormatting sqref="L58">
     <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L56">
+  <conditionalFormatting sqref="L58">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
realisation navbar + page connexion + page inscription + page gestions users + pages gestions annonces
</commit_message>
<xml_diff>
--- a/docs/Analysis/AG_PlanificationProjet.xlsx
+++ b/docs/Analysis/AG_PlanificationProjet.xlsx
@@ -5684,8 +5684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6453,7 +6453,9 @@
       <c r="D32" s="53"/>
       <c r="E32" s="61"/>
       <c r="F32" s="53"/>
-      <c r="G32" s="61"/>
+      <c r="G32" s="61">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H32" s="53"/>
       <c r="I32" s="61"/>
       <c r="J32" s="53"/>
@@ -6462,7 +6464,7 @@
       <c r="M32" s="62"/>
       <c r="N32" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -6616,7 +6618,9 @@
       <c r="C39" s="61"/>
       <c r="D39" s="53"/>
       <c r="E39" s="61"/>
-      <c r="G39" s="53"/>
+      <c r="G39" s="53">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H39" s="61"/>
       <c r="I39" s="61"/>
       <c r="K39" s="53"/>
@@ -6624,7 +6628,7 @@
       <c r="M39" s="62"/>
       <c r="N39" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -6638,7 +6642,9 @@
       <c r="D40" s="53"/>
       <c r="E40" s="61"/>
       <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
+      <c r="G40" s="53">
+        <v>6.25E-2</v>
+      </c>
       <c r="H40" s="61"/>
       <c r="I40" s="53"/>
       <c r="J40" s="61"/>
@@ -6647,7 +6653,7 @@
       <c r="M40" s="62"/>
       <c r="N40" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -6817,7 +6823,9 @@
       <c r="D48" s="53"/>
       <c r="E48" s="61"/>
       <c r="F48" s="53"/>
-      <c r="G48" s="61"/>
+      <c r="G48" s="61">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="I48" s="61"/>
       <c r="J48" s="53"/>
       <c r="K48" s="53"/>
@@ -6825,7 +6833,7 @@
       <c r="M48" s="62"/>
       <c r="N48" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -6861,7 +6869,9 @@
       <c r="D50" s="53"/>
       <c r="E50" s="61"/>
       <c r="F50" s="53"/>
-      <c r="G50" s="61"/>
+      <c r="G50" s="61">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="I50" s="61"/>
       <c r="J50" s="53"/>
       <c r="K50" s="53"/>
@@ -6869,7 +6879,7 @@
       <c r="M50" s="62"/>
       <c r="N50" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -6883,7 +6893,9 @@
       <c r="D51" s="53"/>
       <c r="E51" s="61"/>
       <c r="F51" s="53"/>
-      <c r="G51" s="61"/>
+      <c r="G51" s="61">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I51" s="61"/>
       <c r="J51" s="53"/>
       <c r="K51" s="53"/>
@@ -6891,7 +6903,7 @@
       <c r="M51" s="62"/>
       <c r="N51" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -6905,7 +6917,9 @@
       <c r="D52" s="53"/>
       <c r="E52" s="61"/>
       <c r="F52" s="53"/>
-      <c r="G52" s="61"/>
+      <c r="G52" s="61">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I52" s="61"/>
       <c r="J52" s="53"/>
       <c r="K52" s="53"/>
@@ -6913,7 +6927,7 @@
       <c r="M52" s="62"/>
       <c r="N52" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -6950,7 +6964,9 @@
       <c r="F54" s="61">
         <v>0.10416666666666667</v>
       </c>
-      <c r="G54" s="61"/>
+      <c r="G54" s="61">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H54" s="61">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -6969,7 +6985,7 @@
       </c>
       <c r="N54" s="3">
         <f t="shared" si="0"/>
-        <v>0.5625</v>
+        <v>0.58333333333333326</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -7098,7 +7114,7 @@
       </c>
       <c r="G59" s="77">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H59" s="77">
         <f t="shared" si="1"/>
@@ -7128,11 +7144,11 @@
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M60" s="3">
         <f>SUM(C59:M59)</f>
-        <v>2.208333333333333</v>
+        <v>2.4583333333333326</v>
       </c>
       <c r="N60" s="3">
         <f>SUM(N2:N58)</f>
-        <v>2.1666666666666665</v>
+        <v>2.4166666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
utilisation classe Session + Ajout image Jquery +  Modif Ad Ajax
</commit_message>
<xml_diff>
--- a/docs/Analysis/AG_PlanificationProjet.xlsx
+++ b/docs/Analysis/AG_PlanificationProjet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="81">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>Affichage détails d'une annonce</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -619,7 +616,40 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="333">
+  <dxfs count="337">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4988,690 +5018,690 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F43 H43:I43 I37 I40 G36:G37 H36 H38:H39 D9:D10 H51:I53 F51:F53 G40:G54 I42:I54 L36:L44 E36:E54 C36:C54 E3:E5 E7:E15 C3:C5 C7:C8 I3:I5 I7:I34 G3:G5 G7:G32 L3:L5 L7:L34 C11:C34 E18:E34 L48 L51:L54">
-    <cfRule type="cellIs" dxfId="332" priority="205" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="336" priority="205" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C54 E54:M54 C38:E38 C39:F39 H39 C40:M40 C37:M37 J36:M36 C43:M43 I33:M34 C33:F34 C36:H36 G38:H38 C41:G42 I42 F16:M17 D9:M10 E15:M15 C51:M51 C52:L53 C44:G50 I48:M48 C4:M5 C7:M8 C11:M13 E18:M18 C15:C18 C19:M32 K38:M39 L41:M42 I44:J44 L44 I45:K47 I49:K50">
-    <cfRule type="cellIs" dxfId="331" priority="204" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="335" priority="204" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:K54 F54 H54 M54">
-    <cfRule type="cellIs" dxfId="330" priority="201" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="334" priority="201" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43 G43 J43:K43 J51:K53 G51:G53 D51:D53">
-    <cfRule type="cellIs" dxfId="329" priority="200" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="333" priority="200" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54 E54:M54 C38:E38 C39:F39 H39 C40:M40 C37:M37 J36:M36 C43:M43 I33:M34 C33:F34 C36:H36 G38:H38 C41:G42 I42 F16:M17 C11:M13 D9:M10 C51:M51 C52:L53 C44:G50 I48:M48 C2:M5 C7:M8 E14:M15 E18:M18 C12:C18 C19:M32 K38:M39 L41:M42 I44:J44 L44 I45:K47 I49:K50">
-    <cfRule type="cellIs" dxfId="328" priority="197" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="327" priority="198" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="326" priority="199" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="332" priority="197" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="331" priority="198" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="330" priority="199" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N56">
-    <cfRule type="cellIs" dxfId="325" priority="190" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="329" priority="190" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="324" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="328" priority="196" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="323" priority="192" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="327" priority="192" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="322" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="194" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:M57">
-    <cfRule type="cellIs" dxfId="321" priority="191" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="325" priority="191" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="320" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="324" priority="193" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="319" priority="187" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="323" priority="187" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:J53">
-    <cfRule type="cellIs" dxfId="318" priority="186" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="322" priority="186" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:K53">
-    <cfRule type="cellIs" dxfId="317" priority="185" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="321" priority="185" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E56 C55:C56 G55:G56 I55:I56 L55">
-    <cfRule type="cellIs" dxfId="316" priority="179" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="320" priority="179" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:M55 C56:K56 M56">
-    <cfRule type="cellIs" dxfId="315" priority="178" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="319" priority="178" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:M55 C56:K56 M56">
-    <cfRule type="cellIs" dxfId="314" priority="175" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="313" priority="176" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="312" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="318" priority="175" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="317" priority="176" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="316" priority="177" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="311" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="315" priority="169" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55">
-    <cfRule type="cellIs" dxfId="310" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="314" priority="168" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55">
-    <cfRule type="cellIs" dxfId="309" priority="167" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="313" priority="167" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="308" priority="166" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="312" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="307" priority="163" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="306" priority="164" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="305" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="311" priority="163" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="310" priority="164" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="309" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55">
-    <cfRule type="cellIs" dxfId="304" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="308" priority="162" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="303" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="307" priority="161" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="302" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="306" priority="160" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="301" priority="157" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="300" priority="158" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="299" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="305" priority="157" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="304" priority="158" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="303" priority="159" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="298" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="302" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="297" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="301" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="296" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="300" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44:M45">
-    <cfRule type="cellIs" dxfId="295" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="299" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44:M45">
-    <cfRule type="cellIs" dxfId="294" priority="141" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="293" priority="142" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="292" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="298" priority="141" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="297" priority="142" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="296" priority="143" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46:M47">
-    <cfRule type="cellIs" dxfId="291" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="295" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46:M47">
-    <cfRule type="cellIs" dxfId="290" priority="137" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="289" priority="138" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="288" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="294" priority="137" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="293" priority="138" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="292" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M50">
-    <cfRule type="cellIs" dxfId="287" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="291" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M50">
-    <cfRule type="cellIs" dxfId="286" priority="129" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="285" priority="130" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="284" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="290" priority="129" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="289" priority="130" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="288" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M53">
-    <cfRule type="cellIs" dxfId="283" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="287" priority="128" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M53">
-    <cfRule type="cellIs" dxfId="282" priority="125" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="281" priority="126" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="280" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="286" priority="125" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="285" priority="126" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="284" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52">
-    <cfRule type="cellIs" dxfId="279" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="283" priority="124" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52">
-    <cfRule type="cellIs" dxfId="278" priority="121" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="277" priority="122" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="276" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="282" priority="121" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="281" priority="122" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="280" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35 I35 L35 E35 C35">
-    <cfRule type="cellIs" dxfId="275" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="279" priority="112" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:G35 I35:M35">
-    <cfRule type="cellIs" dxfId="274" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="278" priority="111" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:G35 I35:M35">
-    <cfRule type="cellIs" dxfId="273" priority="108" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="272" priority="109" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="271" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="277" priority="108" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="276" priority="109" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="275" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="270" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="274" priority="100" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="269" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="273" priority="99" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="268" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="272" priority="98" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="267" priority="95" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="266" priority="96" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="265" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="271" priority="95" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="270" priority="96" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="269" priority="97" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="264" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="268" priority="94" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="263" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="267" priority="93" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="262" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="266" priority="92" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="261" priority="91" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="265" priority="91" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="260" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="264" priority="90" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="259" priority="89" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="263" priority="89" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="258" priority="86" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="257" priority="87" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="256" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="262" priority="86" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="261" priority="87" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="260" priority="88" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="255" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="259" priority="85" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="254" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="258" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="253" priority="81" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="252" priority="82" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="251" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="257" priority="81" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="256" priority="82" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="255" priority="83" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="250" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="254" priority="80" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="249" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="253" priority="79" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="248" priority="76" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="77" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="252" priority="76" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="251" priority="77" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="250" priority="78" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="245" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="249" priority="75" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="244" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="248" priority="74" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="243" priority="71" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="242" priority="72" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="73" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="247" priority="71" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="246" priority="72" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="245" priority="73" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="240" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="244" priority="70" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="239" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="243" priority="69" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="238" priority="66" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="67" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="242" priority="66" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="241" priority="67" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="240" priority="68" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="235" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="239" priority="65" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="234" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="238" priority="64" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="233" priority="61" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="232" priority="62" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="237" priority="61" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="236" priority="62" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="235" priority="63" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="230" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="234" priority="60" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="229" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="233" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="228" priority="56" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="57" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="232" priority="56" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="231" priority="57" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="230" priority="58" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="225" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="229" priority="55" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="224" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="228" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="223" priority="51" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="52" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="227" priority="51" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="52" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="225" priority="53" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="220" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="224" priority="50" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="219" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="223" priority="49" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="218" priority="46" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="47" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="222" priority="46" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="221" priority="47" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="220" priority="48" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="215" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="219" priority="45" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="214" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="218" priority="44" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="213" priority="41" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="42" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="217" priority="41" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="216" priority="42" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="215" priority="43" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="210" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="214" priority="40" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="209" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="213" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="208" priority="36" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="37" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="212" priority="36" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="37" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="210" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="205" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="209" priority="35" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="204" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="208" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="203" priority="31" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="32" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="207" priority="31" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="206" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="205" priority="33" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="200" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="204" priority="30" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="199" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="203" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="198" priority="26" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="27" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="202" priority="26" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="201" priority="27" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="200" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="195" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="199" priority="25" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="194" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="198" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="193" priority="21" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="22" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="197" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="195" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="190" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="194" priority="20" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="189" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="193" priority="19" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="188" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="17" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="192" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="191" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="185" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="189" priority="15" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="184" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="188" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="183" priority="11" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="12" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="187" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="186" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="185" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="180" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="184" priority="10" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="179" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="183" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="178" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="182" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="181" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="180" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="175" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="179" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="174" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="178" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="173" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="177" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="175" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5685,7 +5715,7 @@
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6454,7 +6484,7 @@
       <c r="E32" s="61"/>
       <c r="F32" s="53"/>
       <c r="G32" s="61">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="H32" s="53"/>
       <c r="I32" s="61"/>
@@ -6464,7 +6494,7 @@
       <c r="M32" s="62"/>
       <c r="N32" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -6487,7 +6517,10 @@
       <c r="K33" s="53"/>
       <c r="L33" s="61"/>
       <c r="M33" s="62"/>
-      <c r="N33" s="3"/>
+      <c r="N33" s="3">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="45" t="s">
@@ -6502,9 +6535,7 @@
       <c r="F34" s="53">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G34" s="61" t="s">
-        <v>81</v>
-      </c>
+      <c r="G34" s="61"/>
       <c r="H34" s="61"/>
       <c r="I34" s="61"/>
       <c r="J34" s="53"/>
@@ -6528,7 +6559,9 @@
       <c r="E35" s="61"/>
       <c r="F35" s="53"/>
       <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
+      <c r="H35" s="61">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="I35" s="61"/>
       <c r="J35" s="53"/>
       <c r="K35" s="53"/>
@@ -6536,7 +6569,7 @@
       <c r="M35" s="62"/>
       <c r="N35" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -6552,7 +6585,9 @@
       <c r="F36" s="53">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G36" s="61"/>
+      <c r="G36" s="61">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H36" s="53"/>
       <c r="I36" s="61"/>
       <c r="J36" s="53"/>
@@ -6561,7 +6596,7 @@
       <c r="M36" s="62"/>
       <c r="N36" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -6643,7 +6678,7 @@
       <c r="E40" s="61"/>
       <c r="F40" s="53"/>
       <c r="G40" s="53">
-        <v>6.25E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="H40" s="61"/>
       <c r="I40" s="53"/>
@@ -6653,7 +6688,7 @@
       <c r="M40" s="62"/>
       <c r="N40" s="3">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -6688,13 +6723,15 @@
       <c r="D42" s="53"/>
       <c r="E42" s="61"/>
       <c r="F42" s="53"/>
-      <c r="G42" s="61"/>
+      <c r="G42" s="61">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="J42" s="61"/>
       <c r="L42" s="61"/>
       <c r="M42" s="62"/>
       <c r="N42" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -6709,6 +6746,9 @@
       <c r="E43" s="61"/>
       <c r="F43" s="53"/>
       <c r="G43" s="61"/>
+      <c r="H43" s="53">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I43" s="61"/>
       <c r="J43" s="61"/>
       <c r="K43" s="53"/>
@@ -6716,7 +6756,7 @@
       <c r="M43" s="62"/>
       <c r="N43" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -6847,7 +6887,9 @@
       <c r="D49" s="53"/>
       <c r="E49" s="61"/>
       <c r="F49" s="53"/>
-      <c r="G49" s="61"/>
+      <c r="G49" s="61">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="I49" s="61"/>
       <c r="J49" s="53"/>
       <c r="K49" s="53"/>
@@ -6855,7 +6897,7 @@
       <c r="M49" s="62"/>
       <c r="N49" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -6894,7 +6936,7 @@
       <c r="E51" s="61"/>
       <c r="F51" s="53"/>
       <c r="G51" s="61">
-        <v>2.0833333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="I51" s="61"/>
       <c r="J51" s="53"/>
@@ -6903,7 +6945,7 @@
       <c r="M51" s="62"/>
       <c r="N51" s="3">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -7118,7 +7160,7 @@
       </c>
       <c r="H59" s="77">
         <f t="shared" si="1"/>
-        <v>0.125</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I59" s="77">
         <f t="shared" si="1"/>
@@ -7144,699 +7186,715 @@
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M60" s="3">
         <f>SUM(C59:M59)</f>
-        <v>2.4583333333333326</v>
+        <v>2.6666666666666661</v>
       </c>
       <c r="N60" s="3">
         <f>SUM(N2:N58)</f>
-        <v>2.4166666666666665</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:M2 F44 H44:I44 I38 I41 G37:G38 H37 H39:H40 D9:D10 H53:I55 F53:F55 G41:G56 I43 I45:I52 I56 L37:L45 E37:E56 C37:C56 E3:E5 E7:E11 C3:C5 C7:C8 I3:I5 I7:I11 G3:G5 G7:G11 L3:L5 L7:L11 E19:E35 L50 L53:L56 L19:L35 G19:G33 I19:I35 D12:M18 C11:C35 D21:M24">
-    <cfRule type="cellIs" dxfId="170" priority="162" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 F44 H44:I44 I38 I41 G37:G38 H37 H39:H40 D9:D10 H53:I55 F53:F55 I43 I45:I52 I56 L37:L45 E37:E56 C37:C56 E3:E5 E7:E11 C3:C5 C7:C8 I3:I5 I7:I11 G3:G5 G7:G11 L3:L5 L7:L11 E19:E35 L50 L53:L56 L19:L35 G19:G33 I19:I35 D12:M18 C11:C35 D21:M24 G41:G56">
+    <cfRule type="cellIs" dxfId="174" priority="166" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M2 C56 E56:M56 C39:E39 C40:F40 H40 C41:M41 C38:M38 J37:M37 C44:M44 I34:M35 C34:F35 C37:H37 G39:H39 C42:G43 I43 D9:M10 C53:M53 C54:L55 C45:G52 I50:M50 C4:M5 C7:M8 K39:M40 L42:M43 I45:J45 L45 I46:K49 I51:K52 C11:M13 C15:M33">
+  <conditionalFormatting sqref="C2:M2 C56 E56:M56 C39:E39 C40:F40 H40 C41:M41 C38:M38 J37:M37 C44:M44 I34:M35 C34:F35 C37:H37 G39:H39 C42:G43 I43 D9:M10 C53:M53 C54:L55 I50:M50 C4:M5 C7:M8 K39:M40 L42:M43 I45:J45 L45 I46:K49 I51:K52 C11:M13 C15:M33 C45:G52">
+    <cfRule type="cellIs" dxfId="173" priority="165" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J56:K56 F56 H56 M56">
+    <cfRule type="cellIs" dxfId="172" priority="164" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44 G44 J44:K44 J53:K55 G53:G55 D53:D55">
+    <cfRule type="cellIs" dxfId="171" priority="163" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56 E56:M56 C39:E39 C40:F40 H40 C41:M41 C38:M38 J37:M37 C44:M44 I34:M35 C34:F35 C37:H37 G39:H39 C42:G43 I43 D9:M10 C53:M53 C54:L55 I50:M50 C2:M5 C7:M8 K39:M40 L42:M43 I45:J45 L45 I46:K49 I51:K52 C11:M33 C45:G52">
+    <cfRule type="cellIs" dxfId="170" priority="160" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="169" priority="161" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J56:K56 F56 H56 M56">
-    <cfRule type="cellIs" dxfId="168" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="168" priority="162" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N58">
+    <cfRule type="cellIs" dxfId="167" priority="154" operator="greaterThan">
+      <formula>$B2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="159" operator="equal">
+      <formula>$B2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B59">
+    <cfRule type="cellIs" dxfId="165" priority="156" operator="greaterThan">
+      <formula>3.66666666666667</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="158" operator="equal">
+      <formula>3.66666666666667</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:M59">
+    <cfRule type="cellIs" dxfId="163" priority="155" operator="greaterThan">
+      <formula>0.333333333333333</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="162" priority="157" operator="equal">
+      <formula>0.333333333333333</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:M14">
+    <cfRule type="cellIs" dxfId="161" priority="153" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J54:J55">
+    <cfRule type="cellIs" dxfId="160" priority="152" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44 G44 J44:K44 J53:K55 G53:G55 D53:D55">
-    <cfRule type="cellIs" dxfId="167" priority="159" operator="greaterThan">
+  <conditionalFormatting sqref="K54:K55">
+    <cfRule type="cellIs" dxfId="159" priority="151" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56 E56:M56 C39:E39 C40:F40 H40 C41:M41 C38:M38 J37:M37 C44:M44 I34:M35 C34:F35 C37:H37 G39:H39 C42:G43 I43 D9:M10 C53:M53 C54:L55 C45:G52 I50:M50 C2:M5 C7:M8 K39:M40 L42:M43 I45:J45 L45 I46:K49 I51:K52 C11:M33">
-    <cfRule type="cellIs" dxfId="166" priority="156" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="157" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="158" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N58">
-    <cfRule type="cellIs" dxfId="163" priority="150" operator="greaterThan">
-      <formula>$B2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="155" operator="equal">
-      <formula>$B2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
-    <cfRule type="cellIs" dxfId="161" priority="152" operator="greaterThan">
-      <formula>3.66666666666667</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="154" operator="equal">
-      <formula>3.66666666666667</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:M59">
-    <cfRule type="cellIs" dxfId="159" priority="151" operator="greaterThan">
-      <formula>0.333333333333333</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="153" operator="equal">
-      <formula>0.333333333333333</formula>
+  <conditionalFormatting sqref="E57:E58 C57:C58 G57:G58 I57:I58 L57">
+    <cfRule type="cellIs" dxfId="158" priority="150" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:M57 C58:K58 M58">
+    <cfRule type="cellIs" dxfId="157" priority="149" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:M57 C58:K58 M58">
+    <cfRule type="cellIs" dxfId="156" priority="146" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="147" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="148" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57">
+    <cfRule type="cellIs" dxfId="153" priority="145" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J57">
+    <cfRule type="cellIs" dxfId="152" priority="144" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K57">
+    <cfRule type="cellIs" dxfId="151" priority="143" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" dxfId="150" priority="142" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" dxfId="149" priority="139" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="140" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="141" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F57">
+    <cfRule type="cellIs" dxfId="146" priority="138" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="cellIs" dxfId="145" priority="137" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="cellIs" dxfId="144" priority="136" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="cellIs" dxfId="143" priority="133" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="134" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="135" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="157" priority="149" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J54:J55">
-    <cfRule type="cellIs" dxfId="156" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="132" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:M17">
+    <cfRule type="cellIs" dxfId="139" priority="131" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:M17">
+    <cfRule type="cellIs" dxfId="138" priority="130" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M45:M47">
+    <cfRule type="cellIs" dxfId="137" priority="129" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M45:M47">
+    <cfRule type="cellIs" dxfId="136" priority="126" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="135" priority="127" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="128" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M48:M49">
+    <cfRule type="cellIs" dxfId="133" priority="125" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M48:M49">
+    <cfRule type="cellIs" dxfId="132" priority="122" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="123" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="124" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M51:M52">
+    <cfRule type="cellIs" dxfId="129" priority="121" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M51:M52">
+    <cfRule type="cellIs" dxfId="128" priority="118" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="119" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="120" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M55">
+    <cfRule type="cellIs" dxfId="125" priority="117" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M55">
+    <cfRule type="cellIs" dxfId="124" priority="114" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="115" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="116" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M54">
+    <cfRule type="cellIs" dxfId="121" priority="113" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M54">
+    <cfRule type="cellIs" dxfId="120" priority="110" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="111" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="112" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36 I36 L36 E36 C36">
+    <cfRule type="cellIs" dxfId="117" priority="109" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K54:K55">
-    <cfRule type="cellIs" dxfId="155" priority="147" operator="greaterThan">
+  <conditionalFormatting sqref="C36:G36 I36:M36">
+    <cfRule type="cellIs" dxfId="116" priority="108" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:G36 I36:M36">
+    <cfRule type="cellIs" dxfId="115" priority="105" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="106" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="107" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:M14">
+    <cfRule type="cellIs" dxfId="112" priority="104" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="111" priority="103" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E57:E58 C57:C58 G57:G58 I57:I58 L57">
-    <cfRule type="cellIs" dxfId="154" priority="146" operator="greaterThan">
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="110" priority="102" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="109" priority="99" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="100" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="101" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="106" priority="98" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="105" priority="97" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="104" priority="96" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="103" priority="95" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="102" priority="94" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:M57 C58:K58 M58">
-    <cfRule type="cellIs" dxfId="153" priority="145" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:M57 C58:K58 M58">
-    <cfRule type="cellIs" dxfId="152" priority="142" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="143" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="144" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="149" priority="141" operator="greaterThan">
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="101" priority="93" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="100" priority="90" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="91" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="92" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="cellIs" dxfId="97" priority="89" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J57">
-    <cfRule type="cellIs" dxfId="148" priority="140" operator="greaterThan">
+  <conditionalFormatting sqref="H34">
+    <cfRule type="cellIs" dxfId="96" priority="88" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="cellIs" dxfId="95" priority="85" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="86" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="87" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="cellIs" dxfId="92" priority="84" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K57">
-    <cfRule type="cellIs" dxfId="147" priority="139" operator="greaterThan">
+  <conditionalFormatting sqref="H35">
+    <cfRule type="cellIs" dxfId="91" priority="83" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="cellIs" dxfId="90" priority="80" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="81" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="82" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="cellIs" dxfId="87" priority="79" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="cellIs" dxfId="146" priority="138" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="cellIs" dxfId="145" priority="135" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="136" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="137" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F57">
-    <cfRule type="cellIs" dxfId="142" priority="134" operator="greaterThan">
+  <conditionalFormatting sqref="H36">
+    <cfRule type="cellIs" dxfId="86" priority="78" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="cellIs" dxfId="85" priority="75" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="76" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="77" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="cellIs" dxfId="82" priority="74" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="cellIs" dxfId="141" priority="133" operator="greaterThan">
+  <conditionalFormatting sqref="I37">
+    <cfRule type="cellIs" dxfId="81" priority="73" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="cellIs" dxfId="80" priority="70" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="71" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="72" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="cellIs" dxfId="77" priority="69" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="cellIs" dxfId="140" priority="132" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="cellIs" dxfId="139" priority="129" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="130" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="131" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="136" priority="128" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="135" priority="127" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="134" priority="126" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M45:M47">
-    <cfRule type="cellIs" dxfId="133" priority="125" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M45:M47">
-    <cfRule type="cellIs" dxfId="132" priority="122" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="123" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="124" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M48:M49">
-    <cfRule type="cellIs" dxfId="129" priority="121" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M48:M49">
-    <cfRule type="cellIs" dxfId="128" priority="118" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="119" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="120" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M51:M52">
-    <cfRule type="cellIs" dxfId="125" priority="117" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M51:M52">
-    <cfRule type="cellIs" dxfId="124" priority="114" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="115" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="116" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M55">
-    <cfRule type="cellIs" dxfId="121" priority="113" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M55">
-    <cfRule type="cellIs" dxfId="120" priority="110" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="111" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="112" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M54">
-    <cfRule type="cellIs" dxfId="117" priority="109" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M54">
-    <cfRule type="cellIs" dxfId="116" priority="106" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="107" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="108" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G36 I36 L36 E36 C36">
-    <cfRule type="cellIs" dxfId="113" priority="105" operator="greaterThan">
+  <conditionalFormatting sqref="I39">
+    <cfRule type="cellIs" dxfId="76" priority="68" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="cellIs" dxfId="75" priority="65" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="66" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="67" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="cellIs" dxfId="72" priority="64" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:G36 I36:M36">
-    <cfRule type="cellIs" dxfId="112" priority="104" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36:G36 I36:M36">
-    <cfRule type="cellIs" dxfId="111" priority="101" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="102" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="103" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="108" priority="100" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="107" priority="99" operator="greaterThan">
+  <conditionalFormatting sqref="I40">
+    <cfRule type="cellIs" dxfId="71" priority="63" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="cellIs" dxfId="70" priority="60" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="61" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="62" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40">
+    <cfRule type="cellIs" dxfId="67" priority="59" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="106" priority="98" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="105" priority="95" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="96" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="97" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="102" priority="94" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="101" priority="93" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="100" priority="92" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="99" priority="91" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="98" priority="90" operator="greaterThan">
+  <conditionalFormatting sqref="J40">
+    <cfRule type="cellIs" dxfId="66" priority="58" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40">
+    <cfRule type="cellIs" dxfId="65" priority="55" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="56" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="57" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42">
+    <cfRule type="cellIs" dxfId="62" priority="54" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="97" priority="89" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="96" priority="86" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="87" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="88" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="93" priority="85" operator="greaterThan">
+  <conditionalFormatting sqref="J42">
+    <cfRule type="cellIs" dxfId="61" priority="53" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42">
+    <cfRule type="cellIs" dxfId="60" priority="50" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="51" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="52" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K43">
+    <cfRule type="cellIs" dxfId="57" priority="49" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="92" priority="84" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="91" priority="81" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="82" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="83" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="88" priority="80" operator="greaterThan">
+  <conditionalFormatting sqref="K43">
+    <cfRule type="cellIs" dxfId="56" priority="48" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K43">
+    <cfRule type="cellIs" dxfId="55" priority="45" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="46" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="47" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43">
+    <cfRule type="cellIs" dxfId="52" priority="44" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="87" priority="79" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="86" priority="76" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="77" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="78" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="83" priority="75" operator="greaterThan">
+  <conditionalFormatting sqref="J43">
+    <cfRule type="cellIs" dxfId="51" priority="43" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43">
+    <cfRule type="cellIs" dxfId="50" priority="40" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="41" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="42" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K45">
+    <cfRule type="cellIs" dxfId="47" priority="39" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="82" priority="74" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="81" priority="71" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="72" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="73" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="78" priority="70" operator="greaterThan">
+  <conditionalFormatting sqref="K45">
+    <cfRule type="cellIs" dxfId="46" priority="38" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K45">
+    <cfRule type="cellIs" dxfId="45" priority="35" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="36" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="37" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L46:L47">
+    <cfRule type="cellIs" dxfId="42" priority="34" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="77" priority="69" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="76" priority="66" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="67" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="68" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="73" priority="65" operator="greaterThan">
+  <conditionalFormatting sqref="L46:L47">
+    <cfRule type="cellIs" dxfId="41" priority="33" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L46:L47">
+    <cfRule type="cellIs" dxfId="40" priority="30" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="31" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L48">
+    <cfRule type="cellIs" dxfId="37" priority="29" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="72" priority="64" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="71" priority="61" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="62" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="63" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="68" priority="60" operator="greaterThan">
+  <conditionalFormatting sqref="L48">
+    <cfRule type="cellIs" dxfId="36" priority="28" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L48">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="26" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="27" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L49">
+    <cfRule type="cellIs" dxfId="32" priority="24" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="67" priority="59" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="66" priority="56" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="57" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="58" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40">
-    <cfRule type="cellIs" dxfId="63" priority="55" operator="greaterThan">
+  <conditionalFormatting sqref="L49">
+    <cfRule type="cellIs" dxfId="31" priority="23" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L49">
+    <cfRule type="cellIs" dxfId="30" priority="20" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L51">
+    <cfRule type="cellIs" dxfId="27" priority="19" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J40">
-    <cfRule type="cellIs" dxfId="62" priority="54" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40">
-    <cfRule type="cellIs" dxfId="61" priority="51" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="52" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="53" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="58" priority="50" operator="greaterThan">
+  <conditionalFormatting sqref="L51">
+    <cfRule type="cellIs" dxfId="26" priority="18" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L51">
+    <cfRule type="cellIs" dxfId="25" priority="15" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L52">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="57" priority="49" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="56" priority="46" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="47" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="48" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="cellIs" dxfId="53" priority="45" operator="greaterThan">
+  <conditionalFormatting sqref="L52">
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L52">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L58">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="cellIs" dxfId="52" priority="44" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="cellIs" dxfId="51" priority="41" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="42" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="43" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J43">
-    <cfRule type="cellIs" dxfId="48" priority="40" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J43">
-    <cfRule type="cellIs" dxfId="47" priority="39" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J43">
-    <cfRule type="cellIs" dxfId="46" priority="36" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="37" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="38" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45">
-    <cfRule type="cellIs" dxfId="43" priority="35" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45">
-    <cfRule type="cellIs" dxfId="42" priority="34" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45">
-    <cfRule type="cellIs" dxfId="41" priority="31" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="32" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="33" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L46:L47">
-    <cfRule type="cellIs" dxfId="38" priority="30" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L46:L47">
-    <cfRule type="cellIs" dxfId="37" priority="29" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L46:L47">
-    <cfRule type="cellIs" dxfId="36" priority="26" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="27" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="28" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L48">
-    <cfRule type="cellIs" dxfId="33" priority="25" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L48">
-    <cfRule type="cellIs" dxfId="32" priority="24" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L48">
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="28" priority="20" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="27" priority="19" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="17" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="18" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L51">
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L51">
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L51">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L58">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L58">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8574,43 +8632,43 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:L2 F24 H24:I24 C3:C20 E3:E20 G3:G20 I3:I20 K3:K20 C22:C26 G22:G26 I22:I23 I25:I26 E22:E26 K22:K26">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L2 C4:L11 C13:L20 C22:L26">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:L21">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25 F25 H25 J25 L25">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24 G24 J24">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:L26">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ajout fonctionnalite achat + ajout lib dhtmlx et swiftmailer + implementation systeme notif mail
</commit_message>
<xml_diff>
--- a/docs/Analysis/AG_PlanificationProjet.xlsx
+++ b/docs/Analysis/AG_PlanificationProjet.xlsx
@@ -5540,7 +5540,7 @@
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6050,13 +6050,15 @@
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
       <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
+      <c r="J21" s="33">
+        <v>0.125</v>
+      </c>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
       <c r="N21" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -6196,13 +6198,15 @@
       <c r="G27" s="33"/>
       <c r="H27" s="25"/>
       <c r="I27" s="33"/>
-      <c r="J27" s="25"/>
+      <c r="J27" s="25">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="K27" s="25"/>
       <c r="L27" s="33"/>
       <c r="M27" s="34"/>
       <c r="N27" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -6998,7 +7002,7 @@
       </c>
       <c r="J59" s="49">
         <f t="shared" si="1"/>
-        <v>0.125</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K59" s="49">
         <f t="shared" si="1"/>
@@ -7016,11 +7020,11 @@
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M60" s="1">
         <f>SUM(C59:M59)</f>
-        <v>2.9583333333333326</v>
+        <v>3.1666666666666661</v>
       </c>
       <c r="N60" s="1">
         <f>SUM(N2:N58)</f>
-        <v>2.9583333333333339</v>
+        <v>3.166666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction retour fonctions + systeme de mail + creation validation compte + refonte page gestion annonce en ajax
</commit_message>
<xml_diff>
--- a/docs/Analysis/AG_PlanificationProjet.xlsx
+++ b/docs/Analysis/AG_PlanificationProjet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="58">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Affichage détails d'une annonce</t>
+  </si>
+  <si>
+    <t>Affichage des annonces (refonte Ajax)</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,40 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="333">
+  <dxfs count="337">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4843,690 +4879,690 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F43 H43:I43 I37 I40 G36:G37 H36 H38:H39 D9:D10 H51:I53 F51:F53 G40:G54 I42:I54 L36:L44 E36:E54 C36:C54 E3:E5 E7:E15 C3:C5 C7:C8 I3:I5 I7:I34 G3:G5 G7:G32 L3:L5 L7:L34 C11:C34 E18:E34 L48 L51:L54">
-    <cfRule type="cellIs" dxfId="332" priority="205" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="336" priority="205" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C54 E54:M54 C38:E38 C39:F39 H39 C40:M40 C37:M37 J36:M36 C43:M43 I33:M34 C33:F34 C36:H36 G38:H38 C41:G42 I42 F16:M17 D9:M10 E15:M15 C51:M51 C52:L53 C44:G50 I48:M48 C4:M5 C7:M8 C11:M13 E18:M18 C15:C18 C19:M32 K38:M39 L41:M42 I44:J44 L44 I45:K47 I49:K50">
-    <cfRule type="cellIs" dxfId="331" priority="204" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="335" priority="204" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:K54 F54 H54 M54">
-    <cfRule type="cellIs" dxfId="330" priority="201" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="334" priority="201" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43 G43 J43:K43 J51:K53 G51:G53 D51:D53">
-    <cfRule type="cellIs" dxfId="329" priority="200" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="333" priority="200" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54 E54:M54 C38:E38 C39:F39 H39 C40:M40 C37:M37 J36:M36 C43:M43 I33:M34 C33:F34 C36:H36 G38:H38 C41:G42 I42 F16:M17 C11:M13 D9:M10 C51:M51 C52:L53 C44:G50 I48:M48 C2:M5 C7:M8 E14:M15 E18:M18 C12:C18 C19:M32 K38:M39 L41:M42 I44:J44 L44 I45:K47 I49:K50">
-    <cfRule type="cellIs" dxfId="328" priority="197" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="327" priority="198" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="326" priority="199" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="332" priority="197" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="331" priority="198" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="330" priority="199" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N56">
-    <cfRule type="cellIs" dxfId="325" priority="190" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="329" priority="190" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="324" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="328" priority="196" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="323" priority="192" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="327" priority="192" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="322" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="194" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:M57">
-    <cfRule type="cellIs" dxfId="321" priority="191" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="325" priority="191" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="320" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="324" priority="193" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="319" priority="187" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="323" priority="187" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:J53">
-    <cfRule type="cellIs" dxfId="318" priority="186" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="322" priority="186" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:K53">
-    <cfRule type="cellIs" dxfId="317" priority="185" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="321" priority="185" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E56 C55:C56 G55:G56 I55:I56 L55">
-    <cfRule type="cellIs" dxfId="316" priority="179" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="320" priority="179" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:M55 C56:K56 M56">
-    <cfRule type="cellIs" dxfId="315" priority="178" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="319" priority="178" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:M55 C56:K56 M56">
-    <cfRule type="cellIs" dxfId="314" priority="175" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="313" priority="176" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="312" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="318" priority="175" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="317" priority="176" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="316" priority="177" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="311" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="315" priority="169" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55">
-    <cfRule type="cellIs" dxfId="310" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="314" priority="168" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55">
-    <cfRule type="cellIs" dxfId="309" priority="167" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="313" priority="167" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="308" priority="166" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="312" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="307" priority="163" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="306" priority="164" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="305" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="311" priority="163" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="310" priority="164" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="309" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55">
-    <cfRule type="cellIs" dxfId="304" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="308" priority="162" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="303" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="307" priority="161" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="302" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="306" priority="160" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="301" priority="157" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="300" priority="158" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="299" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="305" priority="157" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="304" priority="158" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="303" priority="159" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="298" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="302" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="297" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="301" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="296" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="300" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44:M45">
-    <cfRule type="cellIs" dxfId="295" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="299" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44:M45">
-    <cfRule type="cellIs" dxfId="294" priority="141" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="293" priority="142" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="292" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="298" priority="141" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="297" priority="142" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="296" priority="143" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46:M47">
-    <cfRule type="cellIs" dxfId="291" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="295" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M46:M47">
-    <cfRule type="cellIs" dxfId="290" priority="137" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="289" priority="138" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="288" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="294" priority="137" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="293" priority="138" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="292" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M50">
-    <cfRule type="cellIs" dxfId="287" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="291" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M50">
-    <cfRule type="cellIs" dxfId="286" priority="129" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="285" priority="130" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="284" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="290" priority="129" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="289" priority="130" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="288" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M53">
-    <cfRule type="cellIs" dxfId="283" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="287" priority="128" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M53">
-    <cfRule type="cellIs" dxfId="282" priority="125" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="281" priority="126" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="280" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="286" priority="125" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="285" priority="126" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="284" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52">
-    <cfRule type="cellIs" dxfId="279" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="283" priority="124" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52">
-    <cfRule type="cellIs" dxfId="278" priority="121" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="277" priority="122" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="276" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="282" priority="121" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="281" priority="122" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="280" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35 I35 L35 E35 C35">
-    <cfRule type="cellIs" dxfId="275" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="279" priority="112" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:G35 I35:M35">
-    <cfRule type="cellIs" dxfId="274" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="278" priority="111" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:G35 I35:M35">
-    <cfRule type="cellIs" dxfId="273" priority="108" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="272" priority="109" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="271" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="277" priority="108" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="276" priority="109" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="275" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="270" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="274" priority="100" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="269" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="273" priority="99" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="268" priority="98" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="272" priority="98" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="267" priority="95" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="266" priority="96" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="265" priority="97" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="271" priority="95" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="270" priority="96" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="269" priority="97" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="264" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="268" priority="94" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="263" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="267" priority="93" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="262" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="266" priority="92" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="261" priority="91" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="265" priority="91" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="260" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="264" priority="90" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="259" priority="89" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="263" priority="89" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="258" priority="86" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="257" priority="87" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="256" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="262" priority="86" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="261" priority="87" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="260" priority="88" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="255" priority="85" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="259" priority="85" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="254" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="258" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="253" priority="81" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="252" priority="82" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="251" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="257" priority="81" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="256" priority="82" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="255" priority="83" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="250" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="254" priority="80" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="249" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="253" priority="79" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="248" priority="76" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="77" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="252" priority="76" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="251" priority="77" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="250" priority="78" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="245" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="249" priority="75" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="244" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="248" priority="74" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="243" priority="71" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="242" priority="72" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="73" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="247" priority="71" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="246" priority="72" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="245" priority="73" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="240" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="244" priority="70" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="239" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="243" priority="69" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="238" priority="66" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="67" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="242" priority="66" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="241" priority="67" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="240" priority="68" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="235" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="239" priority="65" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="234" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="238" priority="64" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="233" priority="61" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="232" priority="62" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="237" priority="61" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="236" priority="62" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="235" priority="63" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="230" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="234" priority="60" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="229" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="233" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="228" priority="56" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="57" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="232" priority="56" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="231" priority="57" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="230" priority="58" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="225" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="229" priority="55" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="224" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="228" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="cellIs" dxfId="223" priority="51" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="52" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="227" priority="51" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="52" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="225" priority="53" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="220" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="224" priority="50" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="219" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="223" priority="49" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="cellIs" dxfId="218" priority="46" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="47" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="222" priority="46" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="221" priority="47" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="220" priority="48" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="215" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="219" priority="45" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="214" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="218" priority="44" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="213" priority="41" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="42" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="217" priority="41" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="216" priority="42" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="215" priority="43" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="210" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="214" priority="40" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="209" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="213" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="208" priority="36" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="37" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="212" priority="36" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="37" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="210" priority="38" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="205" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="209" priority="35" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="204" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="208" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="cellIs" dxfId="203" priority="31" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="32" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="207" priority="31" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="206" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="205" priority="33" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="200" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="204" priority="30" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="199" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="203" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="198" priority="26" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="27" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="202" priority="26" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="201" priority="27" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="200" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="195" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="199" priority="25" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="194" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="198" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="193" priority="21" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="22" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="197" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="195" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="190" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="194" priority="20" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="189" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="193" priority="19" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="188" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="17" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="192" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="191" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="185" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="189" priority="15" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="184" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="188" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="183" priority="11" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="12" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="187" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="186" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="185" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="180" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="184" priority="10" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="179" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="183" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="178" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="182" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="181" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="180" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="175" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="179" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="174" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="178" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="173" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="177" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="175" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5540,7 +5576,7 @@
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6053,12 +6089,14 @@
       <c r="J21" s="33">
         <v>0.125</v>
       </c>
-      <c r="K21" s="33"/>
+      <c r="K21" s="33">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
       <c r="N21" s="1">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -6176,12 +6214,14 @@
       <c r="H26" s="25"/>
       <c r="I26" s="33"/>
       <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
+      <c r="K26" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="L26" s="33"/>
       <c r="M26" s="34"/>
       <c r="N26" s="1">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>0.10416666666666666</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -6549,7 +6589,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B42" s="7">
         <v>2.0833333333333332E-2</v>
@@ -6562,11 +6602,14 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="J42" s="33"/>
+      <c r="K42" s="25">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="L42" s="33"/>
       <c r="M42" s="34"/>
       <c r="N42" s="1">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>0.10416666666666666</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -7006,7 +7049,7 @@
       </c>
       <c r="K59" s="49">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="L59" s="49">
         <f t="shared" si="1"/>
@@ -7020,729 +7063,745 @@
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M60" s="1">
         <f>SUM(C59:M59)</f>
-        <v>3.1666666666666661</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="N60" s="1">
         <f>SUM(N2:N58)</f>
-        <v>3.166666666666667</v>
+        <v>3.3333333333333339</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F44 H44:I44 I38 I41 G37:G38 H37 H39:H40 D9:D10 F53:F55 I43 I45:I52 I56 L37:L45 E37:E56 C37:C56 E3:E5 E7:E11 C3:C5 C7:C8 I3:I5 I7:I11 G3:G5 G7:G11 L3:L5 L7:L11 E19:E35 L50 L53:L56 L19:L35 G19:G33 I19:I27 D12:M18 C11:C35 D21:M24 G41:G56 I29:I35 H53:I53 H55:I55 H54 J54">
-    <cfRule type="cellIs" dxfId="170" priority="171" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="174" priority="175" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C56 E56:M56 C39:E39 C40:F40 H40 C41:M41 C38:M38 J37:M37 C44:M44 I34:M35 C34:F35 C37:H37 G39:H39 C42:G43 I43 D9:M10 C53:M53 C55:L55 I50:M50 C4:M5 C7:M8 K39:M40 L42:M43 I45:J45 L45 I46:K49 I51:K52 C11:M13 C15:M27 C45:G52 C29:M33 C28:H28 J28:M28 C54:H54 J54:L54">
+    <cfRule type="cellIs" dxfId="173" priority="174" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J56:K56 F56 H56 M56">
+    <cfRule type="cellIs" dxfId="172" priority="173" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44 G44 J44:K44 J53:K53 G53:G55 D53:D55 J55:K55 K54">
+    <cfRule type="cellIs" dxfId="171" priority="172" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56 E56:M56 C39:E39 C40:F40 H40 C41:M41 C38:M38 J37:M37 C44:M44 I34:M35 C34:F35 C37:H37 G39:H39 C42:G43 I43 D9:M10 C53:M53 C55:L55 I50:M50 C2:M5 C7:M8 K39:M40 L42:M43 I45:J45 L45 I46:K49 I51:K52 C11:M27 C45:G52 C29:M33 C28:H28 J28:M28 C54:H54 J54:L54">
+    <cfRule type="cellIs" dxfId="170" priority="169" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="169" priority="170" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J56:K56 F56 H56 M56">
-    <cfRule type="cellIs" dxfId="168" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="168" priority="171" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N58">
+    <cfRule type="cellIs" dxfId="167" priority="163" operator="greaterThan">
+      <formula>$B2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="168" operator="equal">
+      <formula>$B2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B59">
+    <cfRule type="cellIs" dxfId="165" priority="165" operator="greaterThan">
+      <formula>3.66666666666667</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="167" operator="equal">
+      <formula>3.66666666666667</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:M59">
+    <cfRule type="cellIs" dxfId="163" priority="164" operator="greaterThan">
+      <formula>0.333333333333333</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="162" priority="166" operator="equal">
+      <formula>0.333333333333333</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:M14">
+    <cfRule type="cellIs" dxfId="161" priority="162" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J55">
+    <cfRule type="cellIs" dxfId="160" priority="161" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44 G44 J44:K44 J53:K53 G53:G55 D53:D55 J55:K55 K54">
-    <cfRule type="cellIs" dxfId="167" priority="168" operator="greaterThan">
+  <conditionalFormatting sqref="K54:K55">
+    <cfRule type="cellIs" dxfId="159" priority="160" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56 E56:M56 C39:E39 C40:F40 H40 C41:M41 C38:M38 J37:M37 C44:M44 I34:M35 C34:F35 C37:H37 G39:H39 C42:G43 I43 D9:M10 C53:M53 C55:L55 I50:M50 C2:M5 C7:M8 K39:M40 L42:M43 I45:J45 L45 I46:K49 I51:K52 C11:M27 C45:G52 C29:M33 C28:H28 J28:M28 C54:H54 J54:L54">
-    <cfRule type="cellIs" dxfId="166" priority="165" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="166" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="167" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N58">
-    <cfRule type="cellIs" dxfId="163" priority="159" operator="greaterThan">
-      <formula>$B2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="164" operator="equal">
-      <formula>$B2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
-    <cfRule type="cellIs" dxfId="161" priority="161" operator="greaterThan">
-      <formula>3.66666666666667</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="163" operator="equal">
-      <formula>3.66666666666667</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:M59">
-    <cfRule type="cellIs" dxfId="159" priority="160" operator="greaterThan">
-      <formula>0.333333333333333</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="162" operator="equal">
-      <formula>0.333333333333333</formula>
+  <conditionalFormatting sqref="E57:E58 C57:C58 G57:G58 I57:I58 L57">
+    <cfRule type="cellIs" dxfId="158" priority="159" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:M57 C58:K58 M58">
+    <cfRule type="cellIs" dxfId="157" priority="158" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:M57 C58:K58 M58">
+    <cfRule type="cellIs" dxfId="156" priority="155" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="156" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="157" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57">
+    <cfRule type="cellIs" dxfId="153" priority="154" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J57">
+    <cfRule type="cellIs" dxfId="152" priority="153" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K57">
+    <cfRule type="cellIs" dxfId="151" priority="152" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" dxfId="150" priority="151" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" dxfId="149" priority="148" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="149" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="150" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F57">
+    <cfRule type="cellIs" dxfId="146" priority="147" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="cellIs" dxfId="145" priority="146" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="cellIs" dxfId="144" priority="145" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="cellIs" dxfId="143" priority="142" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="143" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="144" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="157" priority="158" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J55">
-    <cfRule type="cellIs" dxfId="156" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="141" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:M17">
+    <cfRule type="cellIs" dxfId="139" priority="140" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:M17">
+    <cfRule type="cellIs" dxfId="138" priority="139" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M45:M47">
+    <cfRule type="cellIs" dxfId="137" priority="138" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M45:M47">
+    <cfRule type="cellIs" dxfId="136" priority="135" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="135" priority="136" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="137" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M48:M49">
+    <cfRule type="cellIs" dxfId="133" priority="134" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M48:M49">
+    <cfRule type="cellIs" dxfId="132" priority="131" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="132" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="133" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M51:M52">
+    <cfRule type="cellIs" dxfId="129" priority="130" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M51:M52">
+    <cfRule type="cellIs" dxfId="128" priority="127" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="128" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="129" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M55">
+    <cfRule type="cellIs" dxfId="125" priority="126" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M55">
+    <cfRule type="cellIs" dxfId="124" priority="123" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="124" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="125" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M54">
+    <cfRule type="cellIs" dxfId="121" priority="122" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M54">
+    <cfRule type="cellIs" dxfId="120" priority="119" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="120" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="121" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36 I36 L36 E36 C36">
+    <cfRule type="cellIs" dxfId="117" priority="118" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K54:K55">
-    <cfRule type="cellIs" dxfId="155" priority="156" operator="greaterThan">
+  <conditionalFormatting sqref="C36:G36 I36:M36">
+    <cfRule type="cellIs" dxfId="116" priority="117" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:G36 I36:M36">
+    <cfRule type="cellIs" dxfId="115" priority="114" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="115" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="116" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:M14">
+    <cfRule type="cellIs" dxfId="112" priority="113" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="111" priority="112" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E57:E58 C57:C58 G57:G58 I57:I58 L57">
-    <cfRule type="cellIs" dxfId="154" priority="155" operator="greaterThan">
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="110" priority="111" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="109" priority="108" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="109" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="110" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="106" priority="107" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="105" priority="106" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="104" priority="105" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="103" priority="104" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="102" priority="103" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:M57 C58:K58 M58">
-    <cfRule type="cellIs" dxfId="153" priority="154" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:M57 C58:K58 M58">
-    <cfRule type="cellIs" dxfId="152" priority="151" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="152" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="153" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="149" priority="150" operator="greaterThan">
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="101" priority="102" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="100" priority="99" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="100" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="101" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="cellIs" dxfId="97" priority="98" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J57">
-    <cfRule type="cellIs" dxfId="148" priority="149" operator="greaterThan">
+  <conditionalFormatting sqref="H34">
+    <cfRule type="cellIs" dxfId="96" priority="97" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="cellIs" dxfId="95" priority="94" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="95" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="96" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="cellIs" dxfId="92" priority="93" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K57">
-    <cfRule type="cellIs" dxfId="147" priority="148" operator="greaterThan">
+  <conditionalFormatting sqref="H35">
+    <cfRule type="cellIs" dxfId="91" priority="92" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="cellIs" dxfId="90" priority="89" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="90" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="91" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="cellIs" dxfId="87" priority="88" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="cellIs" dxfId="146" priority="147" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="cellIs" dxfId="145" priority="144" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="145" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="146" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F57">
-    <cfRule type="cellIs" dxfId="142" priority="143" operator="greaterThan">
+  <conditionalFormatting sqref="H36">
+    <cfRule type="cellIs" dxfId="86" priority="87" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="cellIs" dxfId="85" priority="84" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="85" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="86" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="cellIs" dxfId="82" priority="83" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="cellIs" dxfId="141" priority="142" operator="greaterThan">
+  <conditionalFormatting sqref="I28">
+    <cfRule type="cellIs" dxfId="81" priority="82" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="cellIs" dxfId="80" priority="79" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="80" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="81" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="cellIs" dxfId="77" priority="78" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="cellIs" dxfId="140" priority="141" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="cellIs" dxfId="139" priority="138" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="139" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="140" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="136" priority="137" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="135" priority="136" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:M17">
-    <cfRule type="cellIs" dxfId="134" priority="135" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M45:M47">
-    <cfRule type="cellIs" dxfId="133" priority="134" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M45:M47">
-    <cfRule type="cellIs" dxfId="132" priority="131" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="132" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="133" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M48:M49">
-    <cfRule type="cellIs" dxfId="129" priority="130" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M48:M49">
-    <cfRule type="cellIs" dxfId="128" priority="127" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="128" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="129" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M51:M52">
-    <cfRule type="cellIs" dxfId="125" priority="126" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M51:M52">
-    <cfRule type="cellIs" dxfId="124" priority="123" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="124" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="125" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M55">
-    <cfRule type="cellIs" dxfId="121" priority="122" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M55">
-    <cfRule type="cellIs" dxfId="120" priority="119" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="120" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="121" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M54">
-    <cfRule type="cellIs" dxfId="117" priority="118" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M54">
-    <cfRule type="cellIs" dxfId="116" priority="115" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="116" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="117" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G36 I36 L36 E36 C36">
-    <cfRule type="cellIs" dxfId="113" priority="114" operator="greaterThan">
+  <conditionalFormatting sqref="I39">
+    <cfRule type="cellIs" dxfId="76" priority="77" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="cellIs" dxfId="75" priority="74" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="75" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="76" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="cellIs" dxfId="72" priority="73" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:G36 I36:M36">
-    <cfRule type="cellIs" dxfId="112" priority="113" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36:G36 I36:M36">
-    <cfRule type="cellIs" dxfId="111" priority="110" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="111" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="112" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:M14">
-    <cfRule type="cellIs" dxfId="108" priority="109" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="107" priority="108" operator="greaterThan">
+  <conditionalFormatting sqref="I40">
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="cellIs" dxfId="70" priority="69" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="71" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40">
+    <cfRule type="cellIs" dxfId="67" priority="68" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="106" priority="107" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="105" priority="104" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="105" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="106" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="102" priority="103" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="101" priority="102" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="100" priority="101" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="99" priority="100" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="98" priority="99" operator="greaterThan">
+  <conditionalFormatting sqref="J40">
+    <cfRule type="cellIs" dxfId="66" priority="67" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40">
+    <cfRule type="cellIs" dxfId="65" priority="64" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="65" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="66" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42">
+    <cfRule type="cellIs" dxfId="62" priority="63" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="97" priority="98" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="96" priority="95" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="96" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="97" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="93" priority="94" operator="greaterThan">
+  <conditionalFormatting sqref="J42">
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42">
+    <cfRule type="cellIs" dxfId="60" priority="59" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="61" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K43">
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="92" priority="93" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="91" priority="90" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="91" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="92" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="88" priority="89" operator="greaterThan">
+  <conditionalFormatting sqref="K43">
+    <cfRule type="cellIs" dxfId="56" priority="57" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K43">
+    <cfRule type="cellIs" dxfId="55" priority="54" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="56" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="87" priority="88" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="86" priority="85" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="86" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="87" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="83" priority="84" operator="greaterThan">
+  <conditionalFormatting sqref="J43">
+    <cfRule type="cellIs" dxfId="51" priority="52" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43">
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K45">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="82" priority="83" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="81" priority="80" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="81" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="82" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="cellIs" dxfId="78" priority="79" operator="greaterThan">
+  <conditionalFormatting sqref="K45">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K45">
+    <cfRule type="cellIs" dxfId="45" priority="44" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="46" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L46:L47">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="cellIs" dxfId="77" priority="78" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="cellIs" dxfId="76" priority="75" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="76" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="77" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="73" priority="74" operator="greaterThan">
+  <conditionalFormatting sqref="L46:L47">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L46:L47">
+    <cfRule type="cellIs" dxfId="40" priority="39" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="41" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L48">
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="72" priority="73" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="cellIs" dxfId="71" priority="70" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="71" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="72" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="68" priority="69" operator="greaterThan">
+  <conditionalFormatting sqref="L48">
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L48">
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="36" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L49">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="67" priority="68" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="66" priority="65" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="66" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="67" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="greaterThan">
+  <conditionalFormatting sqref="L49">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L49">
+    <cfRule type="cellIs" dxfId="30" priority="29" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L51">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J40">
-    <cfRule type="cellIs" dxfId="62" priority="63" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40">
-    <cfRule type="cellIs" dxfId="61" priority="60" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="61" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="62" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="58" priority="59" operator="greaterThan">
+  <conditionalFormatting sqref="L51">
+    <cfRule type="cellIs" dxfId="26" priority="27" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L51">
+    <cfRule type="cellIs" dxfId="25" priority="24" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="26" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L52">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="57" priority="58" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
-    <cfRule type="cellIs" dxfId="56" priority="55" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="56" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="57" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="cellIs" dxfId="53" priority="54" operator="greaterThan">
+  <conditionalFormatting sqref="L52">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L52">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L58">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="cellIs" dxfId="52" priority="53" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="cellIs" dxfId="51" priority="50" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="51" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="52" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J43">
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="greaterThan">
+  <conditionalFormatting sqref="L58">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L58">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J43">
-    <cfRule type="cellIs" dxfId="47" priority="48" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J43">
-    <cfRule type="cellIs" dxfId="46" priority="45" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="47" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45">
-    <cfRule type="cellIs" dxfId="43" priority="44" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45">
-    <cfRule type="cellIs" dxfId="42" priority="43" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45">
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="41" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="42" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L46:L47">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L46:L47">
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L46:L47">
-    <cfRule type="cellIs" dxfId="36" priority="35" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="37" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L48">
-    <cfRule type="cellIs" dxfId="33" priority="34" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L48">
-    <cfRule type="cellIs" dxfId="32" priority="33" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L48">
-    <cfRule type="cellIs" dxfId="31" priority="30" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="31" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="32" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L51">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L51">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L51">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="22" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L58">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L58">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L58">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K42">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
+  <conditionalFormatting sqref="K42">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
doc tables bases + plan navigation + redaction plan de test
</commit_message>
<xml_diff>
--- a/docs/Analysis/AG_PlanificationProjet.xlsx
+++ b/docs/Analysis/AG_PlanificationProjet.xlsx
@@ -5576,7 +5576,7 @@
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6200,7 +6200,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="7">
-        <v>6.25E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="25"/>
@@ -6398,7 +6398,7 @@
         <v>49</v>
       </c>
       <c r="B34" s="7">
-        <v>0.16666666666666666</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C34" s="33"/>
       <c r="D34" s="25"/>
@@ -6592,7 +6592,7 @@
         <v>57</v>
       </c>
       <c r="B42" s="7">
-        <v>2.0833333333333332E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C42" s="33"/>
       <c r="D42" s="25"/>
@@ -6876,7 +6876,7 @@
         <v>30</v>
       </c>
       <c r="B54" s="7">
-        <v>0.58333333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C54" s="33"/>
       <c r="D54" s="33"/>
@@ -6897,14 +6897,14 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L54" s="33">
-        <v>4.1666666666666664E-2</v>
+        <v>0.25</v>
       </c>
       <c r="M54" s="34">
         <v>0.29166666666666669</v>
       </c>
       <c r="N54" s="1">
         <f t="shared" si="0"/>
-        <v>0.58333333333333326</v>
+        <v>0.79166666666666674</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -6958,7 +6958,7 @@
         <v>44</v>
       </c>
       <c r="B57" s="7">
-        <v>0.58333333333333337</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="C57" s="33"/>
       <c r="D57" s="25"/>
@@ -6983,11 +6983,15 @@
       <c r="K57" s="25">
         <v>0.125</v>
       </c>
-      <c r="L57" s="25"/>
-      <c r="M57" s="34"/>
+      <c r="L57" s="25">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M57" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="N57" s="1">
         <f t="shared" si="0"/>
-        <v>0.58333333333333326</v>
+        <v>0.70833333333333326</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7013,7 +7017,7 @@
       <c r="A59" s="48"/>
       <c r="B59" s="49">
         <f>SUM(B2:B58)</f>
-        <v>3.3541666666666674</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="C59" s="49">
         <f t="shared" ref="C59:M59" si="1">SUM(C2:C58)</f>
@@ -7053,21 +7057,21 @@
       </c>
       <c r="L59" s="49">
         <f t="shared" si="1"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M59" s="49">
         <f t="shared" si="1"/>
-        <v>0.29166666666666669</v>
+        <v>0.33333333333333337</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M60" s="1">
         <f>SUM(C59:M59)</f>
-        <v>3.333333333333333</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="N60" s="1">
         <f>SUM(N2:N58)</f>
-        <v>3.3333333333333339</v>
+        <v>3.666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>